<commit_message>
Ajout des résultats, du temps écoulé, et d'un essai de dessin de Lode Runner
</commit_message>
<xml_diff>
--- a/Diagramme_de_Gantt.xlsx
+++ b/Diagramme_de_Gantt.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1247499-FF15-4C84-9993-4885FA6AA47A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{160018D5-DE59-8746-AFCD-303ABBAB6B33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15840" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt" sheetId="11" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="89">
   <si>
     <t>Créez un diagramme de Gantt dans cette feuille de calcul.
 Entrez le titre de ce projet dans la cellule B1. 
@@ -210,9 +210,6 @@
   </si>
   <si>
     <t>Caroline</t>
-  </si>
-  <si>
-    <t>Objectif</t>
   </si>
   <si>
     <t>Mourir dans un trou</t>
@@ -1244,31 +1241,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="7" xfId="9" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="8" xfId="9" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="8" applyFont="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="8" applyBorder="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
     </xf>
@@ -1302,6 +1274,31 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="40" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="8" applyFont="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="8" applyBorder="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="7" xfId="9" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="8" xfId="9" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="50">
@@ -1358,6 +1355,15 @@
   </cellStyles>
   <dxfs count="227">
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor theme="2" tint="-9.9948118533890809E-2"/>
@@ -5604,15 +5610,6 @@
         <vertical/>
         <horizontal/>
       </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <border>
@@ -5876,9 +5873,9 @@
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Description du jalon" dataDxfId="214"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Catégorie" dataDxfId="213"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Affecté à" dataDxfId="212"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Description du jalon" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Catégorie" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Affecté à" dataDxfId="0"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Avancement"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Début" dataCellStyle="Date"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Nombre de jours"/>
@@ -6160,25 +6157,25 @@
   </sheetPr>
   <dimension ref="A1:AB68"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A48" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" style="14" customWidth="1"/>
-    <col min="2" max="2" width="32.42578125" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" style="20" customWidth="1"/>
-    <col min="4" max="4" width="20.42578125" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" customWidth="1"/>
-    <col min="8" max="8" width="2.7109375" customWidth="1"/>
-    <col min="9" max="28" width="9.28515625" customWidth="1"/>
-    <col min="33" max="34" width="10.28515625"/>
+    <col min="1" max="1" width="2.6640625" style="14" customWidth="1"/>
+    <col min="2" max="2" width="32.5" customWidth="1"/>
+    <col min="3" max="3" width="14.83203125" style="20" customWidth="1"/>
+    <col min="4" max="4" width="20.5" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" customWidth="1"/>
+    <col min="6" max="6" width="11.1640625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="10.5" customWidth="1"/>
+    <col min="8" max="8" width="2.6640625" customWidth="1"/>
+    <col min="9" max="28" width="9.33203125" customWidth="1"/>
+    <col min="33" max="34" width="10.33203125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -6212,7 +6209,7 @@
       <c r="AA1" s="20"/>
       <c r="AB1" s="20"/>
     </row>
-    <row r="2" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>1</v>
       </c>
@@ -6222,33 +6219,33 @@
       <c r="C2" s="18"/>
       <c r="F2" s="23"/>
       <c r="G2" s="21"/>
-      <c r="I2" s="56" t="s">
+      <c r="I2" s="71" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="56"/>
-      <c r="K2" s="56"/>
-      <c r="L2" s="56"/>
-      <c r="M2" s="56"/>
-      <c r="O2" s="57" t="s">
+      <c r="J2" s="71"/>
+      <c r="K2" s="71"/>
+      <c r="L2" s="71"/>
+      <c r="M2" s="71"/>
+      <c r="O2" s="72" t="s">
         <v>13</v>
       </c>
-      <c r="P2" s="57"/>
-      <c r="Q2" s="57"/>
-      <c r="R2" s="57"/>
-      <c r="S2" s="57"/>
-      <c r="U2" s="58" t="s">
+      <c r="P2" s="72"/>
+      <c r="Q2" s="72"/>
+      <c r="R2" s="72"/>
+      <c r="S2" s="72"/>
+      <c r="U2" s="73" t="s">
         <v>14</v>
       </c>
-      <c r="V2" s="58"/>
-      <c r="W2" s="58"/>
-      <c r="X2" s="58"/>
-      <c r="Y2" s="58"/>
-      <c r="AA2" s="59" t="s">
+      <c r="V2" s="73"/>
+      <c r="W2" s="73"/>
+      <c r="X2" s="73"/>
+      <c r="Y2" s="73"/>
+      <c r="AA2" s="65" t="s">
         <v>15</v>
       </c>
-      <c r="AB2" s="59"/>
+      <c r="AB2" s="65"/>
     </row>
-    <row r="3" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
         <v>2</v>
       </c>
@@ -6256,24 +6253,24 @@
         <v>49</v>
       </c>
       <c r="C3" s="19"/>
-      <c r="D3" s="60" t="s">
+      <c r="D3" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="61"/>
-      <c r="F3" s="54">
+      <c r="E3" s="67"/>
+      <c r="F3" s="69">
         <v>43880</v>
       </c>
-      <c r="G3" s="55"/>
+      <c r="G3" s="70"/>
       <c r="H3" s="22"/>
     </row>
-    <row r="4" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="60" t="s">
+      <c r="D4" s="66" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="61"/>
+      <c r="E4" s="67"/>
       <c r="F4" s="41">
         <v>0</v>
       </c>
@@ -6307,17 +6304,17 @@
       <c r="AA4" s="40"/>
       <c r="AB4" s="40"/>
     </row>
-    <row r="5" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="53"/>
-      <c r="C5" s="53"/>
-      <c r="D5" s="53"/>
-      <c r="E5" s="53"/>
-      <c r="F5" s="53"/>
-      <c r="G5" s="53"/>
-      <c r="H5" s="53"/>
+      <c r="B5" s="68"/>
+      <c r="C5" s="68"/>
+      <c r="D5" s="68"/>
+      <c r="E5" s="68"/>
+      <c r="F5" s="68"/>
+      <c r="G5" s="68"/>
+      <c r="H5" s="68"/>
       <c r="I5" s="47">
         <f ca="1">IFERROR(Début_Projet+Incrément_Défilement,TODAY())</f>
         <v>43880</v>
@@ -6399,7 +6396,7 @@
         <v>43899</v>
       </c>
     </row>
-    <row r="6" spans="1:28" s="20" customFormat="1" ht="25.35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" s="20" customFormat="1" ht="25.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="s">
         <v>5</v>
       </c>
@@ -6431,7 +6428,7 @@
       <c r="AA6" s="43"/>
       <c r="AB6" s="43"/>
     </row>
-    <row r="7" spans="1:28" ht="30.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:28" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
         <v>6</v>
       </c>
@@ -6535,7 +6532,7 @@
         <v>l</v>
       </c>
     </row>
-    <row r="8" spans="1:28" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:28" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>7</v>
       </c>
@@ -6565,19 +6562,21 @@
       <c r="AA8" s="35"/>
       <c r="AB8" s="35"/>
     </row>
-    <row r="9" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="63" t="s">
+      <c r="B9" s="54" t="s">
         <v>29</v>
       </c>
       <c r="C9" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="20"/>
+        <v>16</v>
+      </c>
+      <c r="D9" s="33" t="s">
+        <v>46</v>
+      </c>
       <c r="E9" s="30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F9" s="51">
         <v>43882</v>
@@ -6667,9 +6666,9 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="15"/>
-      <c r="B10" s="63" t="s">
+      <c r="B10" s="54" t="s">
         <v>30</v>
       </c>
       <c r="C10" s="20"/>
@@ -6761,7 +6760,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="15"/>
       <c r="B11" s="50" t="s">
         <v>31</v>
@@ -6773,7 +6772,7 @@
         <v>46</v>
       </c>
       <c r="E11" s="30">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="F11" s="51">
         <v>43880</v>
@@ -6863,7 +6862,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="14"/>
       <c r="B12" s="50" t="s">
         <v>32</v>
@@ -6875,7 +6874,7 @@
         <v>50</v>
       </c>
       <c r="E12" s="30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F12" s="51">
         <v>43882</v>
@@ -6965,17 +6964,19 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="14"/>
       <c r="B13" s="50" t="s">
         <v>33</v>
       </c>
       <c r="C13" s="33" t="s">
-        <v>51</v>
-      </c>
-      <c r="D13" s="33"/>
+        <v>16</v>
+      </c>
+      <c r="D13" s="33" t="s">
+        <v>50</v>
+      </c>
       <c r="E13" s="30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F13" s="51">
         <v>43882</v>
@@ -6992,9 +6993,9 @@
         <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
-      <c r="K13" s="37">
+      <c r="K13" s="37" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v/>
       </c>
       <c r="L13" s="37" t="str">
         <f t="shared" ca="1" si="5"/>
@@ -7065,9 +7066,9 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="15"/>
-      <c r="B14" s="63" t="s">
+      <c r="B14" s="54" t="s">
         <v>34</v>
       </c>
       <c r="C14" s="20"/>
@@ -7157,15 +7158,19 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="15"/>
       <c r="B15" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="33"/>
-      <c r="D15" s="33"/>
+      <c r="C15" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="33" t="s">
+        <v>50</v>
+      </c>
       <c r="E15" s="30">
-        <v>0</v>
+        <v>0.85</v>
       </c>
       <c r="F15" s="51">
         <v>43882</v>
@@ -7255,12 +7260,14 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="15"/>
       <c r="B16" s="50" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="33"/>
+      <c r="C16" s="33" t="s">
+        <v>13</v>
+      </c>
       <c r="D16" s="33"/>
       <c r="E16" s="30">
         <v>0</v>
@@ -7353,9 +7360,9 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="14"/>
-      <c r="B17" s="63" t="s">
+      <c r="B17" s="54" t="s">
         <v>37</v>
       </c>
       <c r="C17" s="33"/>
@@ -7445,7 +7452,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="14"/>
       <c r="B18" s="50" t="s">
         <v>38</v>
@@ -7537,10 +7544,10 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="14"/>
-      <c r="B19" s="62" t="s">
-        <v>55</v>
+      <c r="B19" s="53" t="s">
+        <v>54</v>
       </c>
       <c r="C19" s="33"/>
       <c r="D19" s="33"/>
@@ -7575,10 +7582,10 @@
       <c r="AA19" s="37"/>
       <c r="AB19" s="37"/>
     </row>
-    <row r="20" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="14"/>
-      <c r="B20" s="62" t="s">
-        <v>56</v>
+      <c r="B20" s="53" t="s">
+        <v>55</v>
       </c>
       <c r="C20" s="33"/>
       <c r="D20" s="33"/>
@@ -7613,7 +7620,7 @@
       <c r="AA20" s="37"/>
       <c r="AB20" s="37"/>
     </row>
-    <row r="21" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="14"/>
       <c r="B21" s="50" t="s">
         <v>39</v>
@@ -7621,94 +7628,94 @@
       <c r="C21" s="33"/>
       <c r="D21" s="33"/>
       <c r="E21" s="30"/>
-      <c r="F21" s="64"/>
+      <c r="F21" s="55"/>
       <c r="G21" s="32"/>
       <c r="H21" s="26"/>
       <c r="I21" s="37" t="str">
-        <f ca="1">IF(AND($C21="Objectif",I$5&gt;=$F22,I$5&lt;=$F22+$G21-1),2,IF(AND($C21="Jalon",I$5&gt;=$F22,I$5&lt;=$F22+$G21-1),1,""))</f>
+        <f t="shared" ref="I21:AB21" ca="1" si="7">IF(AND($C21="Objectif",I$5&gt;=$F22,I$5&lt;=$F22+$G21-1),2,IF(AND($C21="Jalon",I$5&gt;=$F22,I$5&lt;=$F22+$G21-1),1,""))</f>
         <v/>
       </c>
       <c r="J21" s="37" t="str">
-        <f ca="1">IF(AND($C21="Objectif",J$5&gt;=$F22,J$5&lt;=$F22+$G21-1),2,IF(AND($C21="Jalon",J$5&gt;=$F22,J$5&lt;=$F22+$G21-1),1,""))</f>
+        <f t="shared" ca="1" si="7"/>
         <v/>
       </c>
       <c r="K21" s="37" t="str">
-        <f ca="1">IF(AND($C21="Objectif",K$5&gt;=$F22,K$5&lt;=$F22+$G21-1),2,IF(AND($C21="Jalon",K$5&gt;=$F22,K$5&lt;=$F22+$G21-1),1,""))</f>
+        <f t="shared" ca="1" si="7"/>
         <v/>
       </c>
       <c r="L21" s="37" t="str">
-        <f ca="1">IF(AND($C21="Objectif",L$5&gt;=$F22,L$5&lt;=$F22+$G21-1),2,IF(AND($C21="Jalon",L$5&gt;=$F22,L$5&lt;=$F22+$G21-1),1,""))</f>
+        <f t="shared" ca="1" si="7"/>
         <v/>
       </c>
       <c r="M21" s="37" t="str">
-        <f ca="1">IF(AND($C21="Objectif",M$5&gt;=$F22,M$5&lt;=$F22+$G21-1),2,IF(AND($C21="Jalon",M$5&gt;=$F22,M$5&lt;=$F22+$G21-1),1,""))</f>
+        <f t="shared" ca="1" si="7"/>
         <v/>
       </c>
       <c r="N21" s="37" t="str">
-        <f ca="1">IF(AND($C21="Objectif",N$5&gt;=$F22,N$5&lt;=$F22+$G21-1),2,IF(AND($C21="Jalon",N$5&gt;=$F22,N$5&lt;=$F22+$G21-1),1,""))</f>
+        <f t="shared" ca="1" si="7"/>
         <v/>
       </c>
       <c r="O21" s="37" t="str">
-        <f ca="1">IF(AND($C21="Objectif",O$5&gt;=$F22,O$5&lt;=$F22+$G21-1),2,IF(AND($C21="Jalon",O$5&gt;=$F22,O$5&lt;=$F22+$G21-1),1,""))</f>
+        <f t="shared" ca="1" si="7"/>
         <v/>
       </c>
       <c r="P21" s="37" t="str">
-        <f ca="1">IF(AND($C21="Objectif",P$5&gt;=$F22,P$5&lt;=$F22+$G21-1),2,IF(AND($C21="Jalon",P$5&gt;=$F22,P$5&lt;=$F22+$G21-1),1,""))</f>
+        <f t="shared" ca="1" si="7"/>
         <v/>
       </c>
       <c r="Q21" s="37" t="str">
-        <f ca="1">IF(AND($C21="Objectif",Q$5&gt;=$F22,Q$5&lt;=$F22+$G21-1),2,IF(AND($C21="Jalon",Q$5&gt;=$F22,Q$5&lt;=$F22+$G21-1),1,""))</f>
+        <f t="shared" ca="1" si="7"/>
         <v/>
       </c>
       <c r="R21" s="37" t="str">
-        <f ca="1">IF(AND($C21="Objectif",R$5&gt;=$F22,R$5&lt;=$F22+$G21-1),2,IF(AND($C21="Jalon",R$5&gt;=$F22,R$5&lt;=$F22+$G21-1),1,""))</f>
+        <f t="shared" ca="1" si="7"/>
         <v/>
       </c>
       <c r="S21" s="37" t="str">
-        <f ca="1">IF(AND($C21="Objectif",S$5&gt;=$F22,S$5&lt;=$F22+$G21-1),2,IF(AND($C21="Jalon",S$5&gt;=$F22,S$5&lt;=$F22+$G21-1),1,""))</f>
+        <f t="shared" ca="1" si="7"/>
         <v/>
       </c>
       <c r="T21" s="37" t="str">
-        <f ca="1">IF(AND($C21="Objectif",T$5&gt;=$F22,T$5&lt;=$F22+$G21-1),2,IF(AND($C21="Jalon",T$5&gt;=$F22,T$5&lt;=$F22+$G21-1),1,""))</f>
+        <f t="shared" ca="1" si="7"/>
         <v/>
       </c>
       <c r="U21" s="37" t="str">
-        <f ca="1">IF(AND($C21="Objectif",U$5&gt;=$F22,U$5&lt;=$F22+$G21-1),2,IF(AND($C21="Jalon",U$5&gt;=$F22,U$5&lt;=$F22+$G21-1),1,""))</f>
+        <f t="shared" ca="1" si="7"/>
         <v/>
       </c>
       <c r="V21" s="37" t="str">
-        <f ca="1">IF(AND($C21="Objectif",V$5&gt;=$F22,V$5&lt;=$F22+$G21-1),2,IF(AND($C21="Jalon",V$5&gt;=$F22,V$5&lt;=$F22+$G21-1),1,""))</f>
+        <f t="shared" ca="1" si="7"/>
         <v/>
       </c>
       <c r="W21" s="37" t="str">
-        <f ca="1">IF(AND($C21="Objectif",W$5&gt;=$F22,W$5&lt;=$F22+$G21-1),2,IF(AND($C21="Jalon",W$5&gt;=$F22,W$5&lt;=$F22+$G21-1),1,""))</f>
+        <f t="shared" ca="1" si="7"/>
         <v/>
       </c>
       <c r="X21" s="37" t="str">
-        <f ca="1">IF(AND($C21="Objectif",X$5&gt;=$F22,X$5&lt;=$F22+$G21-1),2,IF(AND($C21="Jalon",X$5&gt;=$F22,X$5&lt;=$F22+$G21-1),1,""))</f>
+        <f t="shared" ca="1" si="7"/>
         <v/>
       </c>
       <c r="Y21" s="37" t="str">
-        <f ca="1">IF(AND($C21="Objectif",Y$5&gt;=$F22,Y$5&lt;=$F22+$G21-1),2,IF(AND($C21="Jalon",Y$5&gt;=$F22,Y$5&lt;=$F22+$G21-1),1,""))</f>
+        <f t="shared" ca="1" si="7"/>
         <v/>
       </c>
       <c r="Z21" s="37" t="str">
-        <f ca="1">IF(AND($C21="Objectif",Z$5&gt;=$F22,Z$5&lt;=$F22+$G21-1),2,IF(AND($C21="Jalon",Z$5&gt;=$F22,Z$5&lt;=$F22+$G21-1),1,""))</f>
+        <f t="shared" ca="1" si="7"/>
         <v/>
       </c>
       <c r="AA21" s="37" t="str">
-        <f ca="1">IF(AND($C21="Objectif",AA$5&gt;=$F22,AA$5&lt;=$F22+$G21-1),2,IF(AND($C21="Jalon",AA$5&gt;=$F22,AA$5&lt;=$F22+$G21-1),1,""))</f>
+        <f t="shared" ca="1" si="7"/>
         <v/>
       </c>
       <c r="AB21" s="37" t="str">
-        <f ca="1">IF(AND($C21="Objectif",AB$5&gt;=$F22,AB$5&lt;=$F22+$G21-1),2,IF(AND($C21="Jalon",AB$5&gt;=$F22,AB$5&lt;=$F22+$G21-1),1,""))</f>
+        <f t="shared" ca="1" si="7"/>
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="14"/>
-      <c r="B22" s="62" t="s">
-        <v>57</v>
+      <c r="B22" s="53" t="s">
+        <v>56</v>
       </c>
       <c r="C22" s="33"/>
       <c r="D22" s="33"/>
@@ -7743,102 +7750,102 @@
       <c r="AA22" s="37"/>
       <c r="AB22" s="37"/>
     </row>
-    <row r="23" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="14"/>
       <c r="B23" s="50" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C23" s="33"/>
       <c r="D23" s="33"/>
       <c r="E23" s="30"/>
-      <c r="F23" s="64"/>
+      <c r="F23" s="55"/>
       <c r="G23" s="32"/>
       <c r="H23" s="26"/>
       <c r="I23" s="37" t="str">
-        <f ca="1">IF(AND($C23="Objectif",I$5&gt;=$F24,I$5&lt;=$F24+$G23-1),2,IF(AND($C23="Jalon",I$5&gt;=$F24,I$5&lt;=$F24+$G23-1),1,""))</f>
+        <f t="shared" ref="I23:AB23" ca="1" si="8">IF(AND($C23="Objectif",I$5&gt;=$F24,I$5&lt;=$F24+$G23-1),2,IF(AND($C23="Jalon",I$5&gt;=$F24,I$5&lt;=$F24+$G23-1),1,""))</f>
         <v/>
       </c>
       <c r="J23" s="37" t="str">
-        <f ca="1">IF(AND($C23="Objectif",J$5&gt;=$F24,J$5&lt;=$F24+$G23-1),2,IF(AND($C23="Jalon",J$5&gt;=$F24,J$5&lt;=$F24+$G23-1),1,""))</f>
+        <f t="shared" ca="1" si="8"/>
         <v/>
       </c>
       <c r="K23" s="37" t="str">
-        <f ca="1">IF(AND($C23="Objectif",K$5&gt;=$F24,K$5&lt;=$F24+$G23-1),2,IF(AND($C23="Jalon",K$5&gt;=$F24,K$5&lt;=$F24+$G23-1),1,""))</f>
+        <f t="shared" ca="1" si="8"/>
         <v/>
       </c>
       <c r="L23" s="37" t="str">
-        <f ca="1">IF(AND($C23="Objectif",L$5&gt;=$F24,L$5&lt;=$F24+$G23-1),2,IF(AND($C23="Jalon",L$5&gt;=$F24,L$5&lt;=$F24+$G23-1),1,""))</f>
+        <f t="shared" ca="1" si="8"/>
         <v/>
       </c>
       <c r="M23" s="37" t="str">
-        <f ca="1">IF(AND($C23="Objectif",M$5&gt;=$F24,M$5&lt;=$F24+$G23-1),2,IF(AND($C23="Jalon",M$5&gt;=$F24,M$5&lt;=$F24+$G23-1),1,""))</f>
+        <f t="shared" ca="1" si="8"/>
         <v/>
       </c>
       <c r="N23" s="37" t="str">
-        <f ca="1">IF(AND($C23="Objectif",N$5&gt;=$F24,N$5&lt;=$F24+$G23-1),2,IF(AND($C23="Jalon",N$5&gt;=$F24,N$5&lt;=$F24+$G23-1),1,""))</f>
+        <f t="shared" ca="1" si="8"/>
         <v/>
       </c>
       <c r="O23" s="37" t="str">
-        <f ca="1">IF(AND($C23="Objectif",O$5&gt;=$F24,O$5&lt;=$F24+$G23-1),2,IF(AND($C23="Jalon",O$5&gt;=$F24,O$5&lt;=$F24+$G23-1),1,""))</f>
+        <f t="shared" ca="1" si="8"/>
         <v/>
       </c>
       <c r="P23" s="37" t="str">
-        <f ca="1">IF(AND($C23="Objectif",P$5&gt;=$F24,P$5&lt;=$F24+$G23-1),2,IF(AND($C23="Jalon",P$5&gt;=$F24,P$5&lt;=$F24+$G23-1),1,""))</f>
+        <f t="shared" ca="1" si="8"/>
         <v/>
       </c>
       <c r="Q23" s="37" t="str">
-        <f ca="1">IF(AND($C23="Objectif",Q$5&gt;=$F24,Q$5&lt;=$F24+$G23-1),2,IF(AND($C23="Jalon",Q$5&gt;=$F24,Q$5&lt;=$F24+$G23-1),1,""))</f>
+        <f t="shared" ca="1" si="8"/>
         <v/>
       </c>
       <c r="R23" s="37" t="str">
-        <f ca="1">IF(AND($C23="Objectif",R$5&gt;=$F24,R$5&lt;=$F24+$G23-1),2,IF(AND($C23="Jalon",R$5&gt;=$F24,R$5&lt;=$F24+$G23-1),1,""))</f>
+        <f t="shared" ca="1" si="8"/>
         <v/>
       </c>
       <c r="S23" s="37" t="str">
-        <f ca="1">IF(AND($C23="Objectif",S$5&gt;=$F24,S$5&lt;=$F24+$G23-1),2,IF(AND($C23="Jalon",S$5&gt;=$F24,S$5&lt;=$F24+$G23-1),1,""))</f>
+        <f t="shared" ca="1" si="8"/>
         <v/>
       </c>
       <c r="T23" s="37" t="str">
-        <f ca="1">IF(AND($C23="Objectif",T$5&gt;=$F24,T$5&lt;=$F24+$G23-1),2,IF(AND($C23="Jalon",T$5&gt;=$F24,T$5&lt;=$F24+$G23-1),1,""))</f>
+        <f t="shared" ca="1" si="8"/>
         <v/>
       </c>
       <c r="U23" s="37" t="str">
-        <f ca="1">IF(AND($C23="Objectif",U$5&gt;=$F24,U$5&lt;=$F24+$G23-1),2,IF(AND($C23="Jalon",U$5&gt;=$F24,U$5&lt;=$F24+$G23-1),1,""))</f>
+        <f t="shared" ca="1" si="8"/>
         <v/>
       </c>
       <c r="V23" s="37" t="str">
-        <f ca="1">IF(AND($C23="Objectif",V$5&gt;=$F24,V$5&lt;=$F24+$G23-1),2,IF(AND($C23="Jalon",V$5&gt;=$F24,V$5&lt;=$F24+$G23-1),1,""))</f>
+        <f t="shared" ca="1" si="8"/>
         <v/>
       </c>
       <c r="W23" s="37" t="str">
-        <f ca="1">IF(AND($C23="Objectif",W$5&gt;=$F24,W$5&lt;=$F24+$G23-1),2,IF(AND($C23="Jalon",W$5&gt;=$F24,W$5&lt;=$F24+$G23-1),1,""))</f>
+        <f t="shared" ca="1" si="8"/>
         <v/>
       </c>
       <c r="X23" s="37" t="str">
-        <f ca="1">IF(AND($C23="Objectif",X$5&gt;=$F24,X$5&lt;=$F24+$G23-1),2,IF(AND($C23="Jalon",X$5&gt;=$F24,X$5&lt;=$F24+$G23-1),1,""))</f>
+        <f t="shared" ca="1" si="8"/>
         <v/>
       </c>
       <c r="Y23" s="37" t="str">
-        <f ca="1">IF(AND($C23="Objectif",Y$5&gt;=$F24,Y$5&lt;=$F24+$G23-1),2,IF(AND($C23="Jalon",Y$5&gt;=$F24,Y$5&lt;=$F24+$G23-1),1,""))</f>
+        <f t="shared" ca="1" si="8"/>
         <v/>
       </c>
       <c r="Z23" s="37" t="str">
-        <f ca="1">IF(AND($C23="Objectif",Z$5&gt;=$F24,Z$5&lt;=$F24+$G23-1),2,IF(AND($C23="Jalon",Z$5&gt;=$F24,Z$5&lt;=$F24+$G23-1),1,""))</f>
+        <f t="shared" ca="1" si="8"/>
         <v/>
       </c>
       <c r="AA23" s="37" t="str">
-        <f ca="1">IF(AND($C23="Objectif",AA$5&gt;=$F24,AA$5&lt;=$F24+$G23-1),2,IF(AND($C23="Jalon",AA$5&gt;=$F24,AA$5&lt;=$F24+$G23-1),1,""))</f>
+        <f t="shared" ca="1" si="8"/>
         <v/>
       </c>
       <c r="AB23" s="37" t="str">
-        <f ca="1">IF(AND($C23="Objectif",AB$5&gt;=$F24,AB$5&lt;=$F24+$G23-1),2,IF(AND($C23="Jalon",AB$5&gt;=$F24,AB$5&lt;=$F24+$G23-1),1,""))</f>
+        <f t="shared" ca="1" si="8"/>
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="14"/>
-      <c r="B24" s="62" t="s">
-        <v>58</v>
+      <c r="B24" s="53" t="s">
+        <v>57</v>
       </c>
       <c r="C24" s="33"/>
       <c r="D24" s="33"/>
@@ -7873,10 +7880,10 @@
       <c r="AA24" s="37"/>
       <c r="AB24" s="37"/>
     </row>
-    <row r="25" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="14"/>
-      <c r="B25" s="62" t="s">
-        <v>59</v>
+      <c r="B25" s="53" t="s">
+        <v>58</v>
       </c>
       <c r="C25" s="33"/>
       <c r="D25" s="33"/>
@@ -7911,7 +7918,7 @@
       <c r="AA25" s="37"/>
       <c r="AB25" s="37"/>
     </row>
-    <row r="26" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="14"/>
       <c r="B26" s="50" t="s">
         <v>40</v>
@@ -7927,86 +7934,86 @@
         <v/>
       </c>
       <c r="J26" s="37" t="str">
-        <f t="shared" ref="J26:S52" ca="1" si="7">IF(AND($C26="Objectif",J$5&gt;=$F26,J$5&lt;=$F26+$G26-1),2,IF(AND($C26="Jalon",J$5&gt;=$F26,J$5&lt;=$F26+$G26-1),1,""))</f>
+        <f t="shared" ref="J26:S52" ca="1" si="9">IF(AND($C26="Objectif",J$5&gt;=$F26,J$5&lt;=$F26+$G26-1),2,IF(AND($C26="Jalon",J$5&gt;=$F26,J$5&lt;=$F26+$G26-1),1,""))</f>
         <v/>
       </c>
       <c r="K26" s="37" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="L26" s="37" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="M26" s="37" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="N26" s="37" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="O26" s="37" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="P26" s="37" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="Q26" s="37" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="R26" s="37" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="S26" s="37" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="T26" s="37" t="str">
-        <f t="shared" ref="T26:AB52" ca="1" si="8">IF(AND($C26="Objectif",T$5&gt;=$F26,T$5&lt;=$F26+$G26-1),2,IF(AND($C26="Jalon",T$5&gt;=$F26,T$5&lt;=$F26+$G26-1),1,""))</f>
+        <f t="shared" ref="T26:AB52" ca="1" si="10">IF(AND($C26="Objectif",T$5&gt;=$F26,T$5&lt;=$F26+$G26-1),2,IF(AND($C26="Jalon",T$5&gt;=$F26,T$5&lt;=$F26+$G26-1),1,""))</f>
         <v/>
       </c>
       <c r="U26" s="37" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="10"/>
         <v/>
       </c>
       <c r="V26" s="37" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="10"/>
         <v/>
       </c>
       <c r="W26" s="37" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="10"/>
         <v/>
       </c>
       <c r="X26" s="37" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="10"/>
         <v/>
       </c>
       <c r="Y26" s="37" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="10"/>
         <v/>
       </c>
       <c r="Z26" s="37" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="10"/>
         <v/>
       </c>
       <c r="AA26" s="37" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="10"/>
         <v/>
       </c>
       <c r="AB26" s="37" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="10"/>
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="14"/>
-      <c r="B27" s="62" t="s">
-        <v>61</v>
+      <c r="B27" s="53" t="s">
+        <v>60</v>
       </c>
       <c r="C27" s="33"/>
       <c r="D27" s="33"/>
@@ -8041,10 +8048,10 @@
       <c r="AA27" s="37"/>
       <c r="AB27" s="37"/>
     </row>
-    <row r="28" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="14"/>
-      <c r="B28" s="62" t="s">
-        <v>62</v>
+      <c r="B28" s="53" t="s">
+        <v>61</v>
       </c>
       <c r="C28" s="33"/>
       <c r="D28" s="33"/>
@@ -8079,7 +8086,7 @@
       <c r="AA28" s="37"/>
       <c r="AB28" s="37"/>
     </row>
-    <row r="29" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="14"/>
       <c r="B29" s="50" t="s">
         <v>41</v>
@@ -8101,86 +8108,86 @@
         <v/>
       </c>
       <c r="J29" s="37" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="K29" s="37" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="L29" s="37" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="M29" s="37" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="N29" s="37" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="O29" s="37" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="P29" s="37" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="Q29" s="37" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="R29" s="37" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="S29" s="37" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="T29" s="37" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="10"/>
         <v/>
       </c>
       <c r="U29" s="37" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="10"/>
         <v/>
       </c>
       <c r="V29" s="37" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="10"/>
         <v/>
       </c>
       <c r="W29" s="37" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="10"/>
         <v/>
       </c>
       <c r="X29" s="37" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="10"/>
         <v/>
       </c>
       <c r="Y29" s="37" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="10"/>
         <v/>
       </c>
       <c r="Z29" s="37" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="10"/>
         <v/>
       </c>
       <c r="AA29" s="37" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="10"/>
         <v/>
       </c>
       <c r="AB29" s="37" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="10"/>
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="14"/>
       <c r="B30" s="50" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C30" s="33"/>
       <c r="D30" s="33"/>
@@ -8209,10 +8216,10 @@
       <c r="AA30" s="37"/>
       <c r="AB30" s="37"/>
     </row>
-    <row r="31" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="14"/>
-      <c r="B31" s="62" t="s">
-        <v>52</v>
+      <c r="B31" s="53" t="s">
+        <v>51</v>
       </c>
       <c r="C31" s="33"/>
       <c r="D31" s="33"/>
@@ -8231,123 +8238,123 @@
         <v/>
       </c>
       <c r="J31" s="37" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="K31" s="37" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="L31" s="37" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="M31" s="37" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="N31" s="37" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="O31" s="37" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="P31" s="37" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="Q31" s="37" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="R31" s="37" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="S31" s="37" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="T31" s="37" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="10"/>
         <v/>
       </c>
       <c r="U31" s="37" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="10"/>
         <v/>
       </c>
       <c r="V31" s="37" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="10"/>
         <v/>
       </c>
       <c r="W31" s="37" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="10"/>
         <v/>
       </c>
       <c r="X31" s="37" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="10"/>
         <v/>
       </c>
       <c r="Y31" s="37" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="10"/>
         <v/>
       </c>
       <c r="Z31" s="37" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="10"/>
         <v/>
       </c>
       <c r="AA31" s="37" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="10"/>
         <v/>
       </c>
       <c r="AB31" s="37" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="10"/>
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:28" s="73" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="65"/>
-      <c r="B32" s="66" t="s">
-        <v>54</v>
-      </c>
-      <c r="C32" s="67"/>
-      <c r="D32" s="67"/>
-      <c r="E32" s="68">
+    <row r="32" spans="1:28" s="64" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="56"/>
+      <c r="B32" s="57" t="s">
+        <v>53</v>
+      </c>
+      <c r="C32" s="58"/>
+      <c r="D32" s="58"/>
+      <c r="E32" s="59">
         <v>0</v>
       </c>
-      <c r="F32" s="69">
+      <c r="F32" s="60">
         <v>43894</v>
       </c>
-      <c r="G32" s="70">
+      <c r="G32" s="61">
         <v>2</v>
       </c>
-      <c r="H32" s="71"/>
-      <c r="I32" s="72"/>
-      <c r="J32" s="72"/>
-      <c r="K32" s="72"/>
-      <c r="L32" s="72"/>
-      <c r="M32" s="72"/>
-      <c r="N32" s="72"/>
-      <c r="O32" s="72"/>
-      <c r="P32" s="72"/>
-      <c r="Q32" s="72"/>
-      <c r="R32" s="72"/>
-      <c r="S32" s="72"/>
-      <c r="T32" s="72"/>
-      <c r="U32" s="72"/>
-      <c r="V32" s="72"/>
-      <c r="W32" s="72"/>
-      <c r="X32" s="72"/>
-      <c r="Y32" s="72"/>
-      <c r="Z32" s="72"/>
-      <c r="AA32" s="72"/>
-      <c r="AB32" s="72"/>
+      <c r="H32" s="62"/>
+      <c r="I32" s="63"/>
+      <c r="J32" s="63"/>
+      <c r="K32" s="63"/>
+      <c r="L32" s="63"/>
+      <c r="M32" s="63"/>
+      <c r="N32" s="63"/>
+      <c r="O32" s="63"/>
+      <c r="P32" s="63"/>
+      <c r="Q32" s="63"/>
+      <c r="R32" s="63"/>
+      <c r="S32" s="63"/>
+      <c r="T32" s="63"/>
+      <c r="U32" s="63"/>
+      <c r="V32" s="63"/>
+      <c r="W32" s="63"/>
+      <c r="X32" s="63"/>
+      <c r="Y32" s="63"/>
+      <c r="Z32" s="63"/>
+      <c r="AA32" s="63"/>
+      <c r="AB32" s="63"/>
     </row>
-    <row r="33" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="14"/>
-      <c r="B33" s="63" t="s">
+      <c r="B33" s="54" t="s">
         <v>42</v>
       </c>
       <c r="C33" s="33"/>
@@ -8361,86 +8368,86 @@
         <v/>
       </c>
       <c r="J33" s="37" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="K33" s="37" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="L33" s="37" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="M33" s="37" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="N33" s="37" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="O33" s="37" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="P33" s="37" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="Q33" s="37" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="R33" s="37" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="S33" s="37" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="T33" s="37" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="10"/>
         <v/>
       </c>
       <c r="U33" s="37" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="10"/>
         <v/>
       </c>
       <c r="V33" s="37" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="10"/>
         <v/>
       </c>
       <c r="W33" s="37" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="10"/>
         <v/>
       </c>
       <c r="X33" s="37" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="10"/>
         <v/>
       </c>
       <c r="Y33" s="37" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="10"/>
         <v/>
       </c>
       <c r="Z33" s="37" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="10"/>
         <v/>
       </c>
       <c r="AA33" s="37" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="10"/>
         <v/>
       </c>
       <c r="AB33" s="37" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="10"/>
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="14"/>
       <c r="B34" s="50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C34" s="33"/>
       <c r="D34" s="33"/>
@@ -8475,7 +8482,7 @@
       <c r="AA34" s="37"/>
       <c r="AB34" s="37"/>
     </row>
-    <row r="35" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="14"/>
       <c r="B35" s="50" t="s">
         <v>43</v>
@@ -8487,90 +8494,90 @@
       <c r="G35" s="32"/>
       <c r="H35" s="26"/>
       <c r="I35" s="37" t="str">
-        <f ca="1">IF(AND($C35="Objectif",I$5&gt;=$F36,I$5&lt;=$F36+$G36-1),2,IF(AND($C35="Jalon",I$5&gt;=$F36,I$5&lt;=$F36+$G36-1),1,""))</f>
+        <f t="shared" ref="I35:AB35" ca="1" si="11">IF(AND($C35="Objectif",I$5&gt;=$F36,I$5&lt;=$F36+$G36-1),2,IF(AND($C35="Jalon",I$5&gt;=$F36,I$5&lt;=$F36+$G36-1),1,""))</f>
         <v/>
       </c>
       <c r="J35" s="37" t="str">
-        <f ca="1">IF(AND($C35="Objectif",J$5&gt;=$F36,J$5&lt;=$F36+$G36-1),2,IF(AND($C35="Jalon",J$5&gt;=$F36,J$5&lt;=$F36+$G36-1),1,""))</f>
+        <f t="shared" ca="1" si="11"/>
         <v/>
       </c>
       <c r="K35" s="37" t="str">
-        <f ca="1">IF(AND($C35="Objectif",K$5&gt;=$F36,K$5&lt;=$F36+$G36-1),2,IF(AND($C35="Jalon",K$5&gt;=$F36,K$5&lt;=$F36+$G36-1),1,""))</f>
+        <f t="shared" ca="1" si="11"/>
         <v/>
       </c>
       <c r="L35" s="37" t="str">
-        <f ca="1">IF(AND($C35="Objectif",L$5&gt;=$F36,L$5&lt;=$F36+$G36-1),2,IF(AND($C35="Jalon",L$5&gt;=$F36,L$5&lt;=$F36+$G36-1),1,""))</f>
+        <f t="shared" ca="1" si="11"/>
         <v/>
       </c>
       <c r="M35" s="37" t="str">
-        <f ca="1">IF(AND($C35="Objectif",M$5&gt;=$F36,M$5&lt;=$F36+$G36-1),2,IF(AND($C35="Jalon",M$5&gt;=$F36,M$5&lt;=$F36+$G36-1),1,""))</f>
+        <f t="shared" ca="1" si="11"/>
         <v/>
       </c>
       <c r="N35" s="37" t="str">
-        <f ca="1">IF(AND($C35="Objectif",N$5&gt;=$F36,N$5&lt;=$F36+$G36-1),2,IF(AND($C35="Jalon",N$5&gt;=$F36,N$5&lt;=$F36+$G36-1),1,""))</f>
+        <f t="shared" ca="1" si="11"/>
         <v/>
       </c>
       <c r="O35" s="37" t="str">
-        <f ca="1">IF(AND($C35="Objectif",O$5&gt;=$F36,O$5&lt;=$F36+$G36-1),2,IF(AND($C35="Jalon",O$5&gt;=$F36,O$5&lt;=$F36+$G36-1),1,""))</f>
+        <f t="shared" ca="1" si="11"/>
         <v/>
       </c>
       <c r="P35" s="37" t="str">
-        <f ca="1">IF(AND($C35="Objectif",P$5&gt;=$F36,P$5&lt;=$F36+$G36-1),2,IF(AND($C35="Jalon",P$5&gt;=$F36,P$5&lt;=$F36+$G36-1),1,""))</f>
+        <f t="shared" ca="1" si="11"/>
         <v/>
       </c>
       <c r="Q35" s="37" t="str">
-        <f ca="1">IF(AND($C35="Objectif",Q$5&gt;=$F36,Q$5&lt;=$F36+$G36-1),2,IF(AND($C35="Jalon",Q$5&gt;=$F36,Q$5&lt;=$F36+$G36-1),1,""))</f>
+        <f t="shared" ca="1" si="11"/>
         <v/>
       </c>
       <c r="R35" s="37" t="str">
-        <f ca="1">IF(AND($C35="Objectif",R$5&gt;=$F36,R$5&lt;=$F36+$G36-1),2,IF(AND($C35="Jalon",R$5&gt;=$F36,R$5&lt;=$F36+$G36-1),1,""))</f>
+        <f t="shared" ca="1" si="11"/>
         <v/>
       </c>
       <c r="S35" s="37" t="str">
-        <f ca="1">IF(AND($C35="Objectif",S$5&gt;=$F36,S$5&lt;=$F36+$G36-1),2,IF(AND($C35="Jalon",S$5&gt;=$F36,S$5&lt;=$F36+$G36-1),1,""))</f>
+        <f t="shared" ca="1" si="11"/>
         <v/>
       </c>
       <c r="T35" s="37" t="str">
-        <f ca="1">IF(AND($C35="Objectif",T$5&gt;=$F36,T$5&lt;=$F36+$G36-1),2,IF(AND($C35="Jalon",T$5&gt;=$F36,T$5&lt;=$F36+$G36-1),1,""))</f>
+        <f t="shared" ca="1" si="11"/>
         <v/>
       </c>
       <c r="U35" s="37" t="str">
-        <f ca="1">IF(AND($C35="Objectif",U$5&gt;=$F36,U$5&lt;=$F36+$G36-1),2,IF(AND($C35="Jalon",U$5&gt;=$F36,U$5&lt;=$F36+$G36-1),1,""))</f>
+        <f t="shared" ca="1" si="11"/>
         <v/>
       </c>
       <c r="V35" s="37" t="str">
-        <f ca="1">IF(AND($C35="Objectif",V$5&gt;=$F36,V$5&lt;=$F36+$G36-1),2,IF(AND($C35="Jalon",V$5&gt;=$F36,V$5&lt;=$F36+$G36-1),1,""))</f>
+        <f t="shared" ca="1" si="11"/>
         <v/>
       </c>
       <c r="W35" s="37" t="str">
-        <f ca="1">IF(AND($C35="Objectif",W$5&gt;=$F36,W$5&lt;=$F36+$G36-1),2,IF(AND($C35="Jalon",W$5&gt;=$F36,W$5&lt;=$F36+$G36-1),1,""))</f>
+        <f t="shared" ca="1" si="11"/>
         <v/>
       </c>
       <c r="X35" s="37" t="str">
-        <f ca="1">IF(AND($C35="Objectif",X$5&gt;=$F36,X$5&lt;=$F36+$G36-1),2,IF(AND($C35="Jalon",X$5&gt;=$F36,X$5&lt;=$F36+$G36-1),1,""))</f>
+        <f t="shared" ca="1" si="11"/>
         <v/>
       </c>
       <c r="Y35" s="37" t="str">
-        <f ca="1">IF(AND($C35="Objectif",Y$5&gt;=$F36,Y$5&lt;=$F36+$G36-1),2,IF(AND($C35="Jalon",Y$5&gt;=$F36,Y$5&lt;=$F36+$G36-1),1,""))</f>
+        <f t="shared" ca="1" si="11"/>
         <v/>
       </c>
       <c r="Z35" s="37" t="str">
-        <f ca="1">IF(AND($C35="Objectif",Z$5&gt;=$F36,Z$5&lt;=$F36+$G36-1),2,IF(AND($C35="Jalon",Z$5&gt;=$F36,Z$5&lt;=$F36+$G36-1),1,""))</f>
+        <f t="shared" ca="1" si="11"/>
         <v/>
       </c>
       <c r="AA35" s="37" t="str">
-        <f ca="1">IF(AND($C35="Objectif",AA$5&gt;=$F36,AA$5&lt;=$F36+$G36-1),2,IF(AND($C35="Jalon",AA$5&gt;=$F36,AA$5&lt;=$F36+$G36-1),1,""))</f>
+        <f t="shared" ca="1" si="11"/>
         <v/>
       </c>
       <c r="AB35" s="37" t="str">
-        <f ca="1">IF(AND($C35="Objectif",AB$5&gt;=$F36,AB$5&lt;=$F36+$G36-1),2,IF(AND($C35="Jalon",AB$5&gt;=$F36,AB$5&lt;=$F36+$G36-1),1,""))</f>
+        <f t="shared" ca="1" si="11"/>
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:28" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:28" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="14"/>
-      <c r="B36" s="62" t="s">
-        <v>64</v>
+      <c r="B36" s="53" t="s">
+        <v>63</v>
       </c>
       <c r="C36" s="33"/>
       <c r="D36" s="33"/>
@@ -8605,10 +8612,10 @@
       <c r="AA36" s="37"/>
       <c r="AB36" s="37"/>
     </row>
-    <row r="37" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="14"/>
-      <c r="B37" s="62" t="s">
-        <v>65</v>
+      <c r="B37" s="53" t="s">
+        <v>64</v>
       </c>
       <c r="C37" s="33"/>
       <c r="D37" s="33"/>
@@ -8643,10 +8650,10 @@
       <c r="AA37" s="37"/>
       <c r="AB37" s="37"/>
     </row>
-    <row r="38" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="14"/>
-      <c r="B38" s="62" t="s">
-        <v>73</v>
+      <c r="B38" s="53" t="s">
+        <v>72</v>
       </c>
       <c r="C38" s="33"/>
       <c r="D38" s="33"/>
@@ -8681,7 +8688,7 @@
       <c r="AA38" s="37"/>
       <c r="AB38" s="37"/>
     </row>
-    <row r="39" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="14"/>
       <c r="B39" s="50" t="s">
         <v>44</v>
@@ -8697,86 +8704,86 @@
         <v/>
       </c>
       <c r="J39" s="37" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="K39" s="37" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="L39" s="37" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="M39" s="37" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="N39" s="37" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="O39" s="37" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="P39" s="37" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="Q39" s="37" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="R39" s="37" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="S39" s="37" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="T39" s="37" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="10"/>
         <v/>
       </c>
       <c r="U39" s="37" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="10"/>
         <v/>
       </c>
       <c r="V39" s="37" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="10"/>
         <v/>
       </c>
       <c r="W39" s="37" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="10"/>
         <v/>
       </c>
       <c r="X39" s="37" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="10"/>
         <v/>
       </c>
       <c r="Y39" s="37" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="10"/>
         <v/>
       </c>
       <c r="Z39" s="37" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="10"/>
         <v/>
       </c>
       <c r="AA39" s="37" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="10"/>
         <v/>
       </c>
       <c r="AB39" s="37" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="10"/>
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:28" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:28" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="14"/>
-      <c r="B40" s="62" t="s">
-        <v>66</v>
+      <c r="B40" s="53" t="s">
+        <v>65</v>
       </c>
       <c r="C40" s="33"/>
       <c r="D40" s="33"/>
@@ -8811,10 +8818,10 @@
       <c r="AA40" s="37"/>
       <c r="AB40" s="37"/>
     </row>
-    <row r="41" spans="1:28" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:28" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="14"/>
-      <c r="B41" s="62" t="s">
-        <v>67</v>
+      <c r="B41" s="53" t="s">
+        <v>66</v>
       </c>
       <c r="C41" s="33"/>
       <c r="D41" s="33"/>
@@ -8849,7 +8856,7 @@
       <c r="AA41" s="37"/>
       <c r="AB41" s="37"/>
     </row>
-    <row r="42" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="14"/>
       <c r="B42" s="50" t="s">
         <v>40</v>
@@ -8857,94 +8864,94 @@
       <c r="C42" s="33"/>
       <c r="D42" s="33"/>
       <c r="E42" s="30"/>
-      <c r="F42" s="64"/>
+      <c r="F42" s="55"/>
       <c r="G42" s="32"/>
       <c r="H42" s="26"/>
       <c r="I42" s="37" t="str">
-        <f ca="1">IF(AND($C42="Objectif",I$5&gt;=$F43,I$5&lt;=$F43+$G42-1),2,IF(AND($C42="Jalon",I$5&gt;=$F43,I$5&lt;=$F43+$G42-1),1,""))</f>
+        <f t="shared" ref="I42:AB42" ca="1" si="12">IF(AND($C42="Objectif",I$5&gt;=$F43,I$5&lt;=$F43+$G42-1),2,IF(AND($C42="Jalon",I$5&gt;=$F43,I$5&lt;=$F43+$G42-1),1,""))</f>
         <v/>
       </c>
       <c r="J42" s="37" t="str">
-        <f ca="1">IF(AND($C42="Objectif",J$5&gt;=$F43,J$5&lt;=$F43+$G42-1),2,IF(AND($C42="Jalon",J$5&gt;=$F43,J$5&lt;=$F43+$G42-1),1,""))</f>
+        <f t="shared" ca="1" si="12"/>
         <v/>
       </c>
       <c r="K42" s="37" t="str">
-        <f ca="1">IF(AND($C42="Objectif",K$5&gt;=$F43,K$5&lt;=$F43+$G42-1),2,IF(AND($C42="Jalon",K$5&gt;=$F43,K$5&lt;=$F43+$G42-1),1,""))</f>
+        <f t="shared" ca="1" si="12"/>
         <v/>
       </c>
       <c r="L42" s="37" t="str">
-        <f ca="1">IF(AND($C42="Objectif",L$5&gt;=$F43,L$5&lt;=$F43+$G42-1),2,IF(AND($C42="Jalon",L$5&gt;=$F43,L$5&lt;=$F43+$G42-1),1,""))</f>
+        <f t="shared" ca="1" si="12"/>
         <v/>
       </c>
       <c r="M42" s="37" t="str">
-        <f ca="1">IF(AND($C42="Objectif",M$5&gt;=$F43,M$5&lt;=$F43+$G42-1),2,IF(AND($C42="Jalon",M$5&gt;=$F43,M$5&lt;=$F43+$G42-1),1,""))</f>
+        <f t="shared" ca="1" si="12"/>
         <v/>
       </c>
       <c r="N42" s="37" t="str">
-        <f ca="1">IF(AND($C42="Objectif",N$5&gt;=$F43,N$5&lt;=$F43+$G42-1),2,IF(AND($C42="Jalon",N$5&gt;=$F43,N$5&lt;=$F43+$G42-1),1,""))</f>
+        <f t="shared" ca="1" si="12"/>
         <v/>
       </c>
       <c r="O42" s="37" t="str">
-        <f ca="1">IF(AND($C42="Objectif",O$5&gt;=$F43,O$5&lt;=$F43+$G42-1),2,IF(AND($C42="Jalon",O$5&gt;=$F43,O$5&lt;=$F43+$G42-1),1,""))</f>
+        <f t="shared" ca="1" si="12"/>
         <v/>
       </c>
       <c r="P42" s="37" t="str">
-        <f ca="1">IF(AND($C42="Objectif",P$5&gt;=$F43,P$5&lt;=$F43+$G42-1),2,IF(AND($C42="Jalon",P$5&gt;=$F43,P$5&lt;=$F43+$G42-1),1,""))</f>
+        <f t="shared" ca="1" si="12"/>
         <v/>
       </c>
       <c r="Q42" s="37" t="str">
-        <f ca="1">IF(AND($C42="Objectif",Q$5&gt;=$F43,Q$5&lt;=$F43+$G42-1),2,IF(AND($C42="Jalon",Q$5&gt;=$F43,Q$5&lt;=$F43+$G42-1),1,""))</f>
+        <f t="shared" ca="1" si="12"/>
         <v/>
       </c>
       <c r="R42" s="37" t="str">
-        <f ca="1">IF(AND($C42="Objectif",R$5&gt;=$F43,R$5&lt;=$F43+$G42-1),2,IF(AND($C42="Jalon",R$5&gt;=$F43,R$5&lt;=$F43+$G42-1),1,""))</f>
+        <f t="shared" ca="1" si="12"/>
         <v/>
       </c>
       <c r="S42" s="37" t="str">
-        <f ca="1">IF(AND($C42="Objectif",S$5&gt;=$F43,S$5&lt;=$F43+$G42-1),2,IF(AND($C42="Jalon",S$5&gt;=$F43,S$5&lt;=$F43+$G42-1),1,""))</f>
+        <f t="shared" ca="1" si="12"/>
         <v/>
       </c>
       <c r="T42" s="37" t="str">
-        <f ca="1">IF(AND($C42="Objectif",T$5&gt;=$F43,T$5&lt;=$F43+$G42-1),2,IF(AND($C42="Jalon",T$5&gt;=$F43,T$5&lt;=$F43+$G42-1),1,""))</f>
+        <f t="shared" ca="1" si="12"/>
         <v/>
       </c>
       <c r="U42" s="37" t="str">
-        <f ca="1">IF(AND($C42="Objectif",U$5&gt;=$F43,U$5&lt;=$F43+$G42-1),2,IF(AND($C42="Jalon",U$5&gt;=$F43,U$5&lt;=$F43+$G42-1),1,""))</f>
+        <f t="shared" ca="1" si="12"/>
         <v/>
       </c>
       <c r="V42" s="37" t="str">
-        <f ca="1">IF(AND($C42="Objectif",V$5&gt;=$F43,V$5&lt;=$F43+$G42-1),2,IF(AND($C42="Jalon",V$5&gt;=$F43,V$5&lt;=$F43+$G42-1),1,""))</f>
+        <f t="shared" ca="1" si="12"/>
         <v/>
       </c>
       <c r="W42" s="37" t="str">
-        <f ca="1">IF(AND($C42="Objectif",W$5&gt;=$F43,W$5&lt;=$F43+$G42-1),2,IF(AND($C42="Jalon",W$5&gt;=$F43,W$5&lt;=$F43+$G42-1),1,""))</f>
+        <f t="shared" ca="1" si="12"/>
         <v/>
       </c>
       <c r="X42" s="37" t="str">
-        <f ca="1">IF(AND($C42="Objectif",X$5&gt;=$F43,X$5&lt;=$F43+$G42-1),2,IF(AND($C42="Jalon",X$5&gt;=$F43,X$5&lt;=$F43+$G42-1),1,""))</f>
+        <f t="shared" ca="1" si="12"/>
         <v/>
       </c>
       <c r="Y42" s="37" t="str">
-        <f ca="1">IF(AND($C42="Objectif",Y$5&gt;=$F43,Y$5&lt;=$F43+$G42-1),2,IF(AND($C42="Jalon",Y$5&gt;=$F43,Y$5&lt;=$F43+$G42-1),1,""))</f>
+        <f t="shared" ca="1" si="12"/>
         <v/>
       </c>
       <c r="Z42" s="37" t="str">
-        <f ca="1">IF(AND($C42="Objectif",Z$5&gt;=$F43,Z$5&lt;=$F43+$G42-1),2,IF(AND($C42="Jalon",Z$5&gt;=$F43,Z$5&lt;=$F43+$G42-1),1,""))</f>
+        <f t="shared" ca="1" si="12"/>
         <v/>
       </c>
       <c r="AA42" s="37" t="str">
-        <f ca="1">IF(AND($C42="Objectif",AA$5&gt;=$F43,AA$5&lt;=$F43+$G42-1),2,IF(AND($C42="Jalon",AA$5&gt;=$F43,AA$5&lt;=$F43+$G42-1),1,""))</f>
+        <f t="shared" ca="1" si="12"/>
         <v/>
       </c>
       <c r="AB42" s="37" t="str">
-        <f ca="1">IF(AND($C42="Objectif",AB$5&gt;=$F43,AB$5&lt;=$F43+$G42-1),2,IF(AND($C42="Jalon",AB$5&gt;=$F43,AB$5&lt;=$F43+$G42-1),1,""))</f>
+        <f t="shared" ca="1" si="12"/>
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="14"/>
-      <c r="B43" s="62" t="s">
-        <v>68</v>
+      <c r="B43" s="53" t="s">
+        <v>67</v>
       </c>
       <c r="C43" s="33"/>
       <c r="D43" s="33"/>
@@ -8979,10 +8986,10 @@
       <c r="AA43" s="37"/>
       <c r="AB43" s="37"/>
     </row>
-    <row r="44" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="14"/>
       <c r="B44" s="50" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C44" s="33"/>
       <c r="D44" s="33"/>
@@ -8995,86 +9002,86 @@
         <v/>
       </c>
       <c r="J44" s="37" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="K44" s="37" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="L44" s="37" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="M44" s="37" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="N44" s="37" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="O44" s="37" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="P44" s="37" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="Q44" s="37" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="R44" s="37" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="S44" s="37" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="T44" s="37" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="10"/>
         <v/>
       </c>
       <c r="U44" s="37" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="10"/>
         <v/>
       </c>
       <c r="V44" s="37" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="10"/>
         <v/>
       </c>
       <c r="W44" s="37" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="10"/>
         <v/>
       </c>
       <c r="X44" s="37" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="10"/>
         <v/>
       </c>
       <c r="Y44" s="37" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="10"/>
         <v/>
       </c>
       <c r="Z44" s="37" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="10"/>
         <v/>
       </c>
       <c r="AA44" s="37" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="10"/>
         <v/>
       </c>
       <c r="AB44" s="37" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="10"/>
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:28" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:28" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="14"/>
-      <c r="B45" s="62" t="s">
-        <v>70</v>
+      <c r="B45" s="53" t="s">
+        <v>69</v>
       </c>
       <c r="C45" s="33"/>
       <c r="D45" s="33"/>
@@ -9109,10 +9116,10 @@
       <c r="AA45" s="37"/>
       <c r="AB45" s="37"/>
     </row>
-    <row r="46" spans="1:28" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:28" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="14"/>
-      <c r="B46" s="62" t="s">
-        <v>71</v>
+      <c r="B46" s="53" t="s">
+        <v>70</v>
       </c>
       <c r="C46" s="33"/>
       <c r="D46" s="33"/>
@@ -9147,10 +9154,10 @@
       <c r="AA46" s="37"/>
       <c r="AB46" s="37"/>
     </row>
-    <row r="47" spans="1:28" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:28" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="14"/>
-      <c r="B47" s="62" t="s">
-        <v>72</v>
+      <c r="B47" s="53" t="s">
+        <v>71</v>
       </c>
       <c r="C47" s="33"/>
       <c r="D47" s="33"/>
@@ -9185,10 +9192,10 @@
       <c r="AA47" s="37"/>
       <c r="AB47" s="37"/>
     </row>
-    <row r="48" spans="1:28" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:28" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="14"/>
-      <c r="B48" s="62" t="s">
-        <v>75</v>
+      <c r="B48" s="53" t="s">
+        <v>74</v>
       </c>
       <c r="C48" s="33"/>
       <c r="D48" s="33"/>
@@ -9223,10 +9230,10 @@
       <c r="AA48" s="37"/>
       <c r="AB48" s="37"/>
     </row>
-    <row r="49" spans="1:28" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:28" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="14"/>
-      <c r="B49" s="62" t="s">
-        <v>74</v>
+      <c r="B49" s="53" t="s">
+        <v>73</v>
       </c>
       <c r="C49" s="33"/>
       <c r="D49" s="33"/>
@@ -9261,10 +9268,10 @@
       <c r="AA49" s="37"/>
       <c r="AB49" s="37"/>
     </row>
-    <row r="50" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="14"/>
-      <c r="B50" s="63" t="s">
-        <v>76</v>
+      <c r="B50" s="54" t="s">
+        <v>75</v>
       </c>
       <c r="C50" s="33"/>
       <c r="D50" s="33"/>
@@ -9277,86 +9284,86 @@
         <v/>
       </c>
       <c r="J50" s="37" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="K50" s="37" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="L50" s="37" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="M50" s="37" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="N50" s="37" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="O50" s="37" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="P50" s="37" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="Q50" s="37" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="R50" s="37" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="S50" s="37" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="T50" s="37" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="10"/>
         <v/>
       </c>
       <c r="U50" s="37" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="10"/>
         <v/>
       </c>
       <c r="V50" s="37" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="10"/>
         <v/>
       </c>
       <c r="W50" s="37" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="10"/>
         <v/>
       </c>
       <c r="X50" s="37" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="10"/>
         <v/>
       </c>
       <c r="Y50" s="37" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="10"/>
         <v/>
       </c>
       <c r="Z50" s="37" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="10"/>
         <v/>
       </c>
       <c r="AA50" s="37" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="10"/>
         <v/>
       </c>
       <c r="AB50" s="37" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="10"/>
         <v/>
       </c>
     </row>
-    <row r="51" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="14"/>
       <c r="B51" s="50" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C51" s="33"/>
       <c r="D51" s="33"/>
@@ -9369,86 +9376,86 @@
         <v/>
       </c>
       <c r="J51" s="37" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="K51" s="37" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="L51" s="37" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="M51" s="37" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="N51" s="37" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="O51" s="37" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="P51" s="37" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="Q51" s="37" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="R51" s="37" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="S51" s="37" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="T51" s="37" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="10"/>
         <v/>
       </c>
       <c r="U51" s="37" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="10"/>
         <v/>
       </c>
       <c r="V51" s="37" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="10"/>
         <v/>
       </c>
       <c r="W51" s="37" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="10"/>
         <v/>
       </c>
       <c r="X51" s="37" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="10"/>
         <v/>
       </c>
       <c r="Y51" s="37" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="10"/>
         <v/>
       </c>
       <c r="Z51" s="37" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="10"/>
         <v/>
       </c>
       <c r="AA51" s="37" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="10"/>
         <v/>
       </c>
       <c r="AB51" s="37" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="10"/>
         <v/>
       </c>
     </row>
-    <row r="52" spans="1:28" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:28" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="14"/>
-      <c r="B52" s="62" t="s">
-        <v>78</v>
+      <c r="B52" s="53" t="s">
+        <v>77</v>
       </c>
       <c r="C52" s="33"/>
       <c r="D52" s="33"/>
@@ -9467,86 +9474,86 @@
         <v/>
       </c>
       <c r="J52" s="37" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="K52" s="37" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="L52" s="37" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="M52" s="37" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="N52" s="37" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="O52" s="37" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="P52" s="37" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="Q52" s="37" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="R52" s="37" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="S52" s="37" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="9"/>
         <v/>
       </c>
       <c r="T52" s="37" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="10"/>
         <v/>
       </c>
       <c r="U52" s="37" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="10"/>
         <v/>
       </c>
       <c r="V52" s="37" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="10"/>
         <v/>
       </c>
       <c r="W52" s="37" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="10"/>
         <v/>
       </c>
       <c r="X52" s="37" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="10"/>
         <v/>
       </c>
       <c r="Y52" s="37" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="10"/>
         <v/>
       </c>
       <c r="Z52" s="37" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="10"/>
         <v/>
       </c>
       <c r="AA52" s="37" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="10"/>
         <v/>
       </c>
       <c r="AB52" s="37" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="10"/>
         <v/>
       </c>
     </row>
-    <row r="53" spans="1:28" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:28" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="14"/>
-      <c r="B53" s="62" t="s">
-        <v>79</v>
+      <c r="B53" s="53" t="s">
+        <v>78</v>
       </c>
       <c r="C53" s="33"/>
       <c r="D53" s="33"/>
@@ -9581,102 +9588,102 @@
       <c r="AA53" s="37"/>
       <c r="AB53" s="37"/>
     </row>
-    <row r="54" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="14"/>
       <c r="B54" s="50" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C54" s="33"/>
       <c r="D54" s="33"/>
       <c r="E54" s="30"/>
-      <c r="F54" s="64"/>
+      <c r="F54" s="55"/>
       <c r="G54" s="32"/>
       <c r="H54" s="26"/>
       <c r="I54" s="37" t="str">
-        <f ca="1">IF(AND($C54="Objectif",I$5&gt;=$F55,I$5&lt;=$F55+$G54-1),2,IF(AND($C54="Jalon",I$5&gt;=$F55,I$5&lt;=$F55+$G54-1),1,""))</f>
+        <f t="shared" ref="I54:AB54" ca="1" si="13">IF(AND($C54="Objectif",I$5&gt;=$F55,I$5&lt;=$F55+$G54-1),2,IF(AND($C54="Jalon",I$5&gt;=$F55,I$5&lt;=$F55+$G54-1),1,""))</f>
         <v/>
       </c>
       <c r="J54" s="37" t="str">
-        <f ca="1">IF(AND($C54="Objectif",J$5&gt;=$F55,J$5&lt;=$F55+$G54-1),2,IF(AND($C54="Jalon",J$5&gt;=$F55,J$5&lt;=$F55+$G54-1),1,""))</f>
+        <f t="shared" ca="1" si="13"/>
         <v/>
       </c>
       <c r="K54" s="37" t="str">
-        <f ca="1">IF(AND($C54="Objectif",K$5&gt;=$F55,K$5&lt;=$F55+$G54-1),2,IF(AND($C54="Jalon",K$5&gt;=$F55,K$5&lt;=$F55+$G54-1),1,""))</f>
+        <f t="shared" ca="1" si="13"/>
         <v/>
       </c>
       <c r="L54" s="37" t="str">
-        <f ca="1">IF(AND($C54="Objectif",L$5&gt;=$F55,L$5&lt;=$F55+$G54-1),2,IF(AND($C54="Jalon",L$5&gt;=$F55,L$5&lt;=$F55+$G54-1),1,""))</f>
+        <f t="shared" ca="1" si="13"/>
         <v/>
       </c>
       <c r="M54" s="37" t="str">
-        <f ca="1">IF(AND($C54="Objectif",M$5&gt;=$F55,M$5&lt;=$F55+$G54-1),2,IF(AND($C54="Jalon",M$5&gt;=$F55,M$5&lt;=$F55+$G54-1),1,""))</f>
+        <f t="shared" ca="1" si="13"/>
         <v/>
       </c>
       <c r="N54" s="37" t="str">
-        <f ca="1">IF(AND($C54="Objectif",N$5&gt;=$F55,N$5&lt;=$F55+$G54-1),2,IF(AND($C54="Jalon",N$5&gt;=$F55,N$5&lt;=$F55+$G54-1),1,""))</f>
+        <f t="shared" ca="1" si="13"/>
         <v/>
       </c>
       <c r="O54" s="37" t="str">
-        <f ca="1">IF(AND($C54="Objectif",O$5&gt;=$F55,O$5&lt;=$F55+$G54-1),2,IF(AND($C54="Jalon",O$5&gt;=$F55,O$5&lt;=$F55+$G54-1),1,""))</f>
+        <f t="shared" ca="1" si="13"/>
         <v/>
       </c>
       <c r="P54" s="37" t="str">
-        <f ca="1">IF(AND($C54="Objectif",P$5&gt;=$F55,P$5&lt;=$F55+$G54-1),2,IF(AND($C54="Jalon",P$5&gt;=$F55,P$5&lt;=$F55+$G54-1),1,""))</f>
+        <f t="shared" ca="1" si="13"/>
         <v/>
       </c>
       <c r="Q54" s="37" t="str">
-        <f ca="1">IF(AND($C54="Objectif",Q$5&gt;=$F55,Q$5&lt;=$F55+$G54-1),2,IF(AND($C54="Jalon",Q$5&gt;=$F55,Q$5&lt;=$F55+$G54-1),1,""))</f>
+        <f t="shared" ca="1" si="13"/>
         <v/>
       </c>
       <c r="R54" s="37" t="str">
-        <f ca="1">IF(AND($C54="Objectif",R$5&gt;=$F55,R$5&lt;=$F55+$G54-1),2,IF(AND($C54="Jalon",R$5&gt;=$F55,R$5&lt;=$F55+$G54-1),1,""))</f>
+        <f t="shared" ca="1" si="13"/>
         <v/>
       </c>
       <c r="S54" s="37" t="str">
-        <f ca="1">IF(AND($C54="Objectif",S$5&gt;=$F55,S$5&lt;=$F55+$G54-1),2,IF(AND($C54="Jalon",S$5&gt;=$F55,S$5&lt;=$F55+$G54-1),1,""))</f>
+        <f t="shared" ca="1" si="13"/>
         <v/>
       </c>
       <c r="T54" s="37" t="str">
-        <f ca="1">IF(AND($C54="Objectif",T$5&gt;=$F55,T$5&lt;=$F55+$G54-1),2,IF(AND($C54="Jalon",T$5&gt;=$F55,T$5&lt;=$F55+$G54-1),1,""))</f>
+        <f t="shared" ca="1" si="13"/>
         <v/>
       </c>
       <c r="U54" s="37" t="str">
-        <f ca="1">IF(AND($C54="Objectif",U$5&gt;=$F55,U$5&lt;=$F55+$G54-1),2,IF(AND($C54="Jalon",U$5&gt;=$F55,U$5&lt;=$F55+$G54-1),1,""))</f>
+        <f t="shared" ca="1" si="13"/>
         <v/>
       </c>
       <c r="V54" s="37" t="str">
-        <f ca="1">IF(AND($C54="Objectif",V$5&gt;=$F55,V$5&lt;=$F55+$G54-1),2,IF(AND($C54="Jalon",V$5&gt;=$F55,V$5&lt;=$F55+$G54-1),1,""))</f>
+        <f t="shared" ca="1" si="13"/>
         <v/>
       </c>
       <c r="W54" s="37" t="str">
-        <f ca="1">IF(AND($C54="Objectif",W$5&gt;=$F55,W$5&lt;=$F55+$G54-1),2,IF(AND($C54="Jalon",W$5&gt;=$F55,W$5&lt;=$F55+$G54-1),1,""))</f>
+        <f t="shared" ca="1" si="13"/>
         <v/>
       </c>
       <c r="X54" s="37" t="str">
-        <f ca="1">IF(AND($C54="Objectif",X$5&gt;=$F55,X$5&lt;=$F55+$G54-1),2,IF(AND($C54="Jalon",X$5&gt;=$F55,X$5&lt;=$F55+$G54-1),1,""))</f>
+        <f t="shared" ca="1" si="13"/>
         <v/>
       </c>
       <c r="Y54" s="37" t="str">
-        <f ca="1">IF(AND($C54="Objectif",Y$5&gt;=$F55,Y$5&lt;=$F55+$G54-1),2,IF(AND($C54="Jalon",Y$5&gt;=$F55,Y$5&lt;=$F55+$G54-1),1,""))</f>
+        <f t="shared" ca="1" si="13"/>
         <v/>
       </c>
       <c r="Z54" s="37" t="str">
-        <f ca="1">IF(AND($C54="Objectif",Z$5&gt;=$F55,Z$5&lt;=$F55+$G54-1),2,IF(AND($C54="Jalon",Z$5&gt;=$F55,Z$5&lt;=$F55+$G54-1),1,""))</f>
+        <f t="shared" ca="1" si="13"/>
         <v/>
       </c>
       <c r="AA54" s="37" t="str">
-        <f ca="1">IF(AND($C54="Objectif",AA$5&gt;=$F55,AA$5&lt;=$F55+$G54-1),2,IF(AND($C54="Jalon",AA$5&gt;=$F55,AA$5&lt;=$F55+$G54-1),1,""))</f>
+        <f t="shared" ca="1" si="13"/>
         <v/>
       </c>
       <c r="AB54" s="37" t="str">
-        <f ca="1">IF(AND($C54="Objectif",AB$5&gt;=$F55,AB$5&lt;=$F55+$G54-1),2,IF(AND($C54="Jalon",AB$5&gt;=$F55,AB$5&lt;=$F55+$G54-1),1,""))</f>
+        <f t="shared" ca="1" si="13"/>
         <v/>
       </c>
     </row>
-    <row r="55" spans="1:28" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:28" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="14"/>
-      <c r="B55" s="62" t="s">
-        <v>80</v>
+      <c r="B55" s="53" t="s">
+        <v>79</v>
       </c>
       <c r="C55" s="33"/>
       <c r="D55" s="33"/>
@@ -9711,10 +9718,10 @@
       <c r="AA55" s="37"/>
       <c r="AB55" s="37"/>
     </row>
-    <row r="56" spans="1:28" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:28" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="14"/>
-      <c r="B56" s="62" t="s">
-        <v>82</v>
+      <c r="B56" s="53" t="s">
+        <v>81</v>
       </c>
       <c r="C56" s="33"/>
       <c r="D56" s="33"/>
@@ -9749,21 +9756,25 @@
       <c r="AA56" s="37"/>
       <c r="AB56" s="37"/>
     </row>
-    <row r="57" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="14"/>
       <c r="B57" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="C57" s="33"/>
-      <c r="D57" s="33"/>
+      <c r="C57" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="D57" s="33" t="s">
+        <v>50</v>
+      </c>
       <c r="E57" s="30">
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="F57" s="51">
         <v>43882</v>
       </c>
       <c r="G57" s="32">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H57" s="26"/>
       <c r="I57" s="37"/>
@@ -9787,10 +9798,10 @@
       <c r="AA57" s="37"/>
       <c r="AB57" s="37"/>
     </row>
-    <row r="58" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="14"/>
       <c r="B58" s="50" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C58" s="33"/>
       <c r="D58" s="33"/>
@@ -9819,10 +9830,10 @@
       <c r="AA58" s="37"/>
       <c r="AB58" s="37"/>
     </row>
-    <row r="59" spans="1:28" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:28" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="14"/>
-      <c r="B59" s="62" t="s">
-        <v>84</v>
+      <c r="B59" s="53" t="s">
+        <v>83</v>
       </c>
       <c r="C59" s="33"/>
       <c r="D59" s="33"/>
@@ -9857,10 +9868,10 @@
       <c r="AA59" s="37"/>
       <c r="AB59" s="37"/>
     </row>
-    <row r="60" spans="1:28" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:28" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="14"/>
-      <c r="B60" s="62" t="s">
-        <v>85</v>
+      <c r="B60" s="53" t="s">
+        <v>84</v>
       </c>
       <c r="C60" s="33"/>
       <c r="D60" s="33"/>
@@ -9895,10 +9906,10 @@
       <c r="AA60" s="37"/>
       <c r="AB60" s="37"/>
     </row>
-    <row r="61" spans="1:28" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:28" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="14"/>
-      <c r="B61" s="62" t="s">
-        <v>86</v>
+      <c r="B61" s="53" t="s">
+        <v>85</v>
       </c>
       <c r="C61" s="33"/>
       <c r="D61" s="33"/>
@@ -9933,10 +9944,10 @@
       <c r="AA61" s="37"/>
       <c r="AB61" s="37"/>
     </row>
-    <row r="62" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="14"/>
       <c r="B62" s="50" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C62" s="33"/>
       <c r="D62" s="33"/>
@@ -9965,10 +9976,10 @@
       <c r="AA62" s="37"/>
       <c r="AB62" s="37"/>
     </row>
-    <row r="63" spans="1:28" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:28" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="14"/>
-      <c r="B63" s="62" t="s">
-        <v>88</v>
+      <c r="B63" s="53" t="s">
+        <v>87</v>
       </c>
       <c r="C63" s="33"/>
       <c r="D63" s="33"/>
@@ -10003,10 +10014,10 @@
       <c r="AA63" s="37"/>
       <c r="AB63" s="37"/>
     </row>
-    <row r="64" spans="1:28" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:28" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="14"/>
-      <c r="B64" s="62" t="s">
-        <v>89</v>
+      <c r="B64" s="53" t="s">
+        <v>88</v>
       </c>
       <c r="C64" s="33"/>
       <c r="D64" s="33"/>
@@ -10041,7 +10052,7 @@
       <c r="AA64" s="37"/>
       <c r="AB64" s="37"/>
     </row>
-    <row r="65" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="14"/>
       <c r="B65" s="50"/>
       <c r="C65" s="33"/>
@@ -10071,7 +10082,7 @@
       <c r="AA65" s="37"/>
       <c r="AB65" s="37"/>
     </row>
-    <row r="66" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A66" s="15" t="s">
         <v>9</v>
       </c>
@@ -10105,12 +10116,12 @@
       <c r="AA66" s="36"/>
       <c r="AB66" s="36"/>
     </row>
-    <row r="67" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D67" s="5"/>
       <c r="G67" s="16"/>
       <c r="H67" s="4"/>
     </row>
-    <row r="68" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D68" s="6"/>
     </row>
   </sheetData>
@@ -10139,44 +10150,44 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5:AA13 I16:AA16 I18:AA18 I31:AA31 I21:AA21 I23:AA23 I66:AA66">
-    <cfRule type="expression" dxfId="211" priority="613">
+    <cfRule type="expression" dxfId="214" priority="613">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4:AB4">
-    <cfRule type="expression" dxfId="210" priority="619">
+    <cfRule type="expression" dxfId="213" priority="619">
       <formula>I$5&lt;=EOMONTH($I$5,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:AB4">
-    <cfRule type="expression" dxfId="209" priority="615">
+    <cfRule type="expression" dxfId="212" priority="615">
       <formula>AND(J$5&lt;=EOMONTH($I$5,2),J$5&gt;EOMONTH($I$5,0),J$5&gt;EOMONTH($I$5,1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4:AB4">
-    <cfRule type="expression" dxfId="208" priority="614">
+    <cfRule type="expression" dxfId="211" priority="614">
       <formula>AND(I$5&lt;=EOMONTH($I$5,1),I$5&gt;EOMONTH($I$5,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8:AB13 I16:AB16 I18:AB18 I26:AB26 I29:AB33 I39:AB39 I44:AB44 I50:AB51 I56:AB57">
-    <cfRule type="expression" dxfId="207" priority="636" stopIfTrue="1">
+    <cfRule type="expression" dxfId="210" priority="636" stopIfTrue="1">
       <formula>AND($C8="Risque faible",I$5&gt;=$F8,I$5&lt;=$F8+$G8-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="206" priority="655" stopIfTrue="1">
+    <cfRule type="expression" dxfId="209" priority="655" stopIfTrue="1">
       <formula>AND($C8="Risque élevé",I$5&gt;=$F8,I$5&lt;=$F8+$G8-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="205" priority="673" stopIfTrue="1">
+    <cfRule type="expression" dxfId="208" priority="673" stopIfTrue="1">
       <formula>AND($C8="En bonne voie",I$5&gt;=$F8,I$5&lt;=$F8+$G8-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="204" priority="674" stopIfTrue="1">
+    <cfRule type="expression" dxfId="207" priority="674" stopIfTrue="1">
       <formula>AND($C8="Risque moyen",I$5&gt;=$F8,I$5&lt;=$F8+$G8-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="203" priority="675" stopIfTrue="1">
+    <cfRule type="expression" dxfId="206" priority="675" stopIfTrue="1">
       <formula>AND(LEN($C8)=0,I$5&gt;=$F8,I$5&lt;=$F8+$G8-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB5:AB13 AB16 AB18 AB31 AB21 AB23 AB66">
-    <cfRule type="expression" dxfId="202" priority="684">
+    <cfRule type="expression" dxfId="205" priority="684">
       <formula>AND(TODAY()&gt;=AB$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10209,29 +10220,29 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I14:AA14">
-    <cfRule type="expression" dxfId="201" priority="595">
+    <cfRule type="expression" dxfId="204" priority="595">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I14:AB14">
-    <cfRule type="expression" dxfId="200" priority="597" stopIfTrue="1">
+    <cfRule type="expression" dxfId="203" priority="597" stopIfTrue="1">
       <formula>AND($C14="Risque faible",I$5&gt;=$F14,I$5&lt;=$F14+$G14-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="199" priority="598" stopIfTrue="1">
+    <cfRule type="expression" dxfId="202" priority="598" stopIfTrue="1">
       <formula>AND($C14="Risque élevé",I$5&gt;=$F14,I$5&lt;=$F14+$G14-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="198" priority="599" stopIfTrue="1">
+    <cfRule type="expression" dxfId="201" priority="599" stopIfTrue="1">
       <formula>AND($C14="En bonne voie",I$5&gt;=$F14,I$5&lt;=$F14+$G14-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="197" priority="600" stopIfTrue="1">
+    <cfRule type="expression" dxfId="200" priority="600" stopIfTrue="1">
       <formula>AND($C14="Risque moyen",I$5&gt;=$F14,I$5&lt;=$F14+$G14-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="196" priority="601" stopIfTrue="1">
+    <cfRule type="expression" dxfId="199" priority="601" stopIfTrue="1">
       <formula>AND(LEN($C14)=0,I$5&gt;=$F14,I$5&lt;=$F14+$G14-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB14">
-    <cfRule type="expression" dxfId="195" priority="602">
+    <cfRule type="expression" dxfId="198" priority="602">
       <formula>AND(TODAY()&gt;=AB$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10250,29 +10261,29 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I15:AA15">
-    <cfRule type="expression" dxfId="194" priority="586">
+    <cfRule type="expression" dxfId="197" priority="586">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I15:AB15">
-    <cfRule type="expression" dxfId="193" priority="588" stopIfTrue="1">
+    <cfRule type="expression" dxfId="196" priority="588" stopIfTrue="1">
       <formula>AND($C15="Risque faible",I$5&gt;=$F15,I$5&lt;=$F15+$G15-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="192" priority="589" stopIfTrue="1">
+    <cfRule type="expression" dxfId="195" priority="589" stopIfTrue="1">
       <formula>AND($C15="Risque élevé",I$5&gt;=$F15,I$5&lt;=$F15+$G15-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="191" priority="590" stopIfTrue="1">
+    <cfRule type="expression" dxfId="194" priority="590" stopIfTrue="1">
       <formula>AND($C15="En bonne voie",I$5&gt;=$F15,I$5&lt;=$F15+$G15-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="190" priority="591" stopIfTrue="1">
+    <cfRule type="expression" dxfId="193" priority="591" stopIfTrue="1">
       <formula>AND($C15="Risque moyen",I$5&gt;=$F15,I$5&lt;=$F15+$G15-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="189" priority="592" stopIfTrue="1">
+    <cfRule type="expression" dxfId="192" priority="592" stopIfTrue="1">
       <formula>AND(LEN($C15)=0,I$5&gt;=$F15,I$5&lt;=$F15+$G15-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB15">
-    <cfRule type="expression" dxfId="188" priority="593">
+    <cfRule type="expression" dxfId="191" priority="593">
       <formula>AND(TODAY()&gt;=AB$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10291,29 +10302,29 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I17:AA17">
-    <cfRule type="expression" dxfId="187" priority="577">
+    <cfRule type="expression" dxfId="190" priority="577">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I17:AB17">
-    <cfRule type="expression" dxfId="186" priority="579" stopIfTrue="1">
+    <cfRule type="expression" dxfId="189" priority="579" stopIfTrue="1">
       <formula>AND($C17="Risque faible",I$5&gt;=$F17,I$5&lt;=$F17+$G17-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="185" priority="580" stopIfTrue="1">
+    <cfRule type="expression" dxfId="188" priority="580" stopIfTrue="1">
       <formula>AND($C17="Risque élevé",I$5&gt;=$F17,I$5&lt;=$F17+$G17-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="184" priority="581" stopIfTrue="1">
+    <cfRule type="expression" dxfId="187" priority="581" stopIfTrue="1">
       <formula>AND($C17="En bonne voie",I$5&gt;=$F17,I$5&lt;=$F17+$G17-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="183" priority="582" stopIfTrue="1">
+    <cfRule type="expression" dxfId="186" priority="582" stopIfTrue="1">
       <formula>AND($C17="Risque moyen",I$5&gt;=$F17,I$5&lt;=$F17+$G17-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="182" priority="583" stopIfTrue="1">
+    <cfRule type="expression" dxfId="185" priority="583" stopIfTrue="1">
       <formula>AND(LEN($C17)=0,I$5&gt;=$F17,I$5&lt;=$F17+$G17-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB17">
-    <cfRule type="expression" dxfId="181" priority="584">
+    <cfRule type="expression" dxfId="184" priority="584">
       <formula>AND(TODAY()&gt;=AB$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10332,12 +10343,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I26:AA26">
-    <cfRule type="expression" dxfId="180" priority="568">
+    <cfRule type="expression" dxfId="183" priority="568">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB26">
-    <cfRule type="expression" dxfId="179" priority="575">
+    <cfRule type="expression" dxfId="182" priority="575">
       <formula>AND(TODAY()&gt;=AB$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10356,12 +10367,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I29:AA29">
-    <cfRule type="expression" dxfId="178" priority="559">
+    <cfRule type="expression" dxfId="181" priority="559">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB29">
-    <cfRule type="expression" dxfId="177" priority="566">
+    <cfRule type="expression" dxfId="180" priority="566">
       <formula>AND(TODAY()&gt;=AB$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10380,42 +10391,42 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I33:AA33">
-    <cfRule type="expression" dxfId="176" priority="550">
+    <cfRule type="expression" dxfId="179" priority="550">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB33">
-    <cfRule type="expression" dxfId="175" priority="557">
+    <cfRule type="expression" dxfId="178" priority="557">
       <formula>AND(TODAY()&gt;=AB$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I39:AA39 I42:AA42 I44:AA44">
-    <cfRule type="expression" dxfId="174" priority="532">
+    <cfRule type="expression" dxfId="177" priority="532">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB39 AB42 AB44">
-    <cfRule type="expression" dxfId="173" priority="539">
+    <cfRule type="expression" dxfId="176" priority="539">
       <formula>AND(TODAY()&gt;=AB$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I54:AA54">
-    <cfRule type="expression" dxfId="172" priority="514">
+    <cfRule type="expression" dxfId="175" priority="514">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB54">
-    <cfRule type="expression" dxfId="171" priority="521">
+    <cfRule type="expression" dxfId="174" priority="521">
       <formula>AND(TODAY()&gt;=AB$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I57:AA57">
-    <cfRule type="expression" dxfId="170" priority="505">
+    <cfRule type="expression" dxfId="173" priority="505">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB57">
-    <cfRule type="expression" dxfId="169" priority="512">
+    <cfRule type="expression" dxfId="172" priority="512">
       <formula>AND(TODAY()&gt;=AB$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10504,22 +10515,22 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I50:AA50">
-    <cfRule type="expression" dxfId="168" priority="489">
+    <cfRule type="expression" dxfId="171" priority="489">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB50">
-    <cfRule type="expression" dxfId="167" priority="496">
+    <cfRule type="expression" dxfId="170" priority="496">
       <formula>AND(TODAY()&gt;=AB$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I51:AA51">
-    <cfRule type="expression" dxfId="166" priority="481">
+    <cfRule type="expression" dxfId="169" priority="481">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB51">
-    <cfRule type="expression" dxfId="165" priority="487">
+    <cfRule type="expression" dxfId="168" priority="487">
       <formula>AND(TODAY()&gt;=AB$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10552,12 +10563,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I30:AA30">
-    <cfRule type="expression" dxfId="164" priority="471">
+    <cfRule type="expression" dxfId="167" priority="471">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB30">
-    <cfRule type="expression" dxfId="163" priority="478">
+    <cfRule type="expression" dxfId="166" priority="478">
       <formula>AND(TODAY()&gt;=AB$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10576,12 +10587,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I32:AA32">
-    <cfRule type="expression" dxfId="162" priority="462">
+    <cfRule type="expression" dxfId="165" priority="462">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB32">
-    <cfRule type="expression" dxfId="161" priority="469">
+    <cfRule type="expression" dxfId="164" priority="469">
       <formula>AND(TODAY()&gt;=AB$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10600,46 +10611,46 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I19:AA19">
-    <cfRule type="expression" dxfId="160" priority="453">
+    <cfRule type="expression" dxfId="163" priority="453">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I19:AB19">
-    <cfRule type="expression" dxfId="159" priority="455" stopIfTrue="1">
+    <cfRule type="expression" dxfId="162" priority="455" stopIfTrue="1">
       <formula>AND($C19="Risque faible",I$5&gt;=$F19,I$5&lt;=$F19+$G19-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="158" priority="456" stopIfTrue="1">
+    <cfRule type="expression" dxfId="161" priority="456" stopIfTrue="1">
       <formula>AND($C19="Risque élevé",I$5&gt;=$F19,I$5&lt;=$F19+$G19-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="157" priority="457" stopIfTrue="1">
+    <cfRule type="expression" dxfId="160" priority="457" stopIfTrue="1">
       <formula>AND($C19="En bonne voie",I$5&gt;=$F19,I$5&lt;=$F19+$G19-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="156" priority="458" stopIfTrue="1">
+    <cfRule type="expression" dxfId="159" priority="458" stopIfTrue="1">
       <formula>AND($C19="Risque moyen",I$5&gt;=$F19,I$5&lt;=$F19+$G19-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="155" priority="459" stopIfTrue="1">
+    <cfRule type="expression" dxfId="158" priority="459" stopIfTrue="1">
       <formula>AND(LEN($C19)=0,I$5&gt;=$F19,I$5&lt;=$F19+$G19-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB19">
-    <cfRule type="expression" dxfId="154" priority="460">
+    <cfRule type="expression" dxfId="157" priority="460">
       <formula>AND(TODAY()&gt;=AB$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I21:AB21 I23:AB23 I42:AB42 I54:AB54">
-    <cfRule type="expression" dxfId="153" priority="738" stopIfTrue="1">
+    <cfRule type="expression" dxfId="156" priority="738" stopIfTrue="1">
       <formula>AND($C21="Risque faible",I$5&gt;=$F22,I$5&lt;=$F22+$G21-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="152" priority="739" stopIfTrue="1">
+    <cfRule type="expression" dxfId="155" priority="739" stopIfTrue="1">
       <formula>AND($C21="Risque élevé",I$5&gt;=$F22,I$5&lt;=$F22+$G21-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="151" priority="740" stopIfTrue="1">
+    <cfRule type="expression" dxfId="154" priority="740" stopIfTrue="1">
       <formula>AND($C21="En bonne voie",I$5&gt;=$F22,I$5&lt;=$F22+$G21-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="150" priority="741" stopIfTrue="1">
+    <cfRule type="expression" dxfId="153" priority="741" stopIfTrue="1">
       <formula>AND($C21="Risque moyen",I$5&gt;=$F22,I$5&lt;=$F22+$G21-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="149" priority="742" stopIfTrue="1">
+    <cfRule type="expression" dxfId="152" priority="742" stopIfTrue="1">
       <formula>AND(LEN($C21)=0,I$5&gt;=$F22,I$5&lt;=$F22+$G21-1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10658,29 +10669,29 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I34:AA34">
-    <cfRule type="expression" dxfId="148" priority="381">
+    <cfRule type="expression" dxfId="151" priority="381">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I34:AB34">
-    <cfRule type="expression" dxfId="147" priority="383" stopIfTrue="1">
+    <cfRule type="expression" dxfId="150" priority="383" stopIfTrue="1">
       <formula>AND($C34="Risque faible",I$5&gt;=$F34,I$5&lt;=$F34+$G34-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="146" priority="384" stopIfTrue="1">
+    <cfRule type="expression" dxfId="149" priority="384" stopIfTrue="1">
       <formula>AND($C34="Risque élevé",I$5&gt;=$F34,I$5&lt;=$F34+$G34-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="145" priority="385" stopIfTrue="1">
+    <cfRule type="expression" dxfId="148" priority="385" stopIfTrue="1">
       <formula>AND($C34="En bonne voie",I$5&gt;=$F34,I$5&lt;=$F34+$G34-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="144" priority="386" stopIfTrue="1">
+    <cfRule type="expression" dxfId="147" priority="386" stopIfTrue="1">
       <formula>AND($C34="Risque moyen",I$5&gt;=$F34,I$5&lt;=$F34+$G34-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="143" priority="387" stopIfTrue="1">
+    <cfRule type="expression" dxfId="146" priority="387" stopIfTrue="1">
       <formula>AND(LEN($C34)=0,I$5&gt;=$F34,I$5&lt;=$F34+$G34-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB34">
-    <cfRule type="expression" dxfId="142" priority="388">
+    <cfRule type="expression" dxfId="145" priority="388">
       <formula>AND(TODAY()&gt;=AB$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10699,7 +10710,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I22:AA22">
-    <cfRule type="expression" dxfId="141" priority="335">
+    <cfRule type="expression" dxfId="144" priority="335">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10718,29 +10729,29 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I27:AA28">
-    <cfRule type="expression" dxfId="140" priority="353">
+    <cfRule type="expression" dxfId="143" priority="353">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I27:AB28">
-    <cfRule type="expression" dxfId="139" priority="355" stopIfTrue="1">
+    <cfRule type="expression" dxfId="142" priority="355" stopIfTrue="1">
       <formula>AND($C27="Risque faible",I$5&gt;=$F27,I$5&lt;=$F27+$G27-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="138" priority="356" stopIfTrue="1">
+    <cfRule type="expression" dxfId="141" priority="356" stopIfTrue="1">
       <formula>AND($C27="Risque élevé",I$5&gt;=$F27,I$5&lt;=$F27+$G27-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="137" priority="357" stopIfTrue="1">
+    <cfRule type="expression" dxfId="140" priority="357" stopIfTrue="1">
       <formula>AND($C27="En bonne voie",I$5&gt;=$F27,I$5&lt;=$F27+$G27-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="136" priority="358" stopIfTrue="1">
+    <cfRule type="expression" dxfId="139" priority="358" stopIfTrue="1">
       <formula>AND($C27="Risque moyen",I$5&gt;=$F27,I$5&lt;=$F27+$G27-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="135" priority="359" stopIfTrue="1">
+    <cfRule type="expression" dxfId="138" priority="359" stopIfTrue="1">
       <formula>AND(LEN($C27)=0,I$5&gt;=$F27,I$5&lt;=$F27+$G27-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB27:AB28">
-    <cfRule type="expression" dxfId="134" priority="360">
+    <cfRule type="expression" dxfId="137" priority="360">
       <formula>AND(TODAY()&gt;=AB$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10759,51 +10770,51 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I24:AA25">
-    <cfRule type="expression" dxfId="133" priority="344">
+    <cfRule type="expression" dxfId="136" priority="344">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I24:AB25">
-    <cfRule type="expression" dxfId="132" priority="346" stopIfTrue="1">
+    <cfRule type="expression" dxfId="135" priority="346" stopIfTrue="1">
       <formula>AND($C24="Risque faible",I$5&gt;=$F24,I$5&lt;=$F24+$G24-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="131" priority="347" stopIfTrue="1">
+    <cfRule type="expression" dxfId="134" priority="347" stopIfTrue="1">
       <formula>AND($C24="Risque élevé",I$5&gt;=$F24,I$5&lt;=$F24+$G24-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="130" priority="348" stopIfTrue="1">
+    <cfRule type="expression" dxfId="133" priority="348" stopIfTrue="1">
       <formula>AND($C24="En bonne voie",I$5&gt;=$F24,I$5&lt;=$F24+$G24-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="129" priority="349" stopIfTrue="1">
+    <cfRule type="expression" dxfId="132" priority="349" stopIfTrue="1">
       <formula>AND($C24="Risque moyen",I$5&gt;=$F24,I$5&lt;=$F24+$G24-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="128" priority="350" stopIfTrue="1">
+    <cfRule type="expression" dxfId="131" priority="350" stopIfTrue="1">
       <formula>AND(LEN($C24)=0,I$5&gt;=$F24,I$5&lt;=$F24+$G24-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB24:AB25">
-    <cfRule type="expression" dxfId="127" priority="351">
+    <cfRule type="expression" dxfId="130" priority="351">
       <formula>AND(TODAY()&gt;=AB$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I22:AB22">
-    <cfRule type="expression" dxfId="126" priority="337" stopIfTrue="1">
+    <cfRule type="expression" dxfId="129" priority="337" stopIfTrue="1">
       <formula>AND($C22="Risque faible",I$5&gt;=$F22,I$5&lt;=$F22+$G22-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="125" priority="338" stopIfTrue="1">
+    <cfRule type="expression" dxfId="128" priority="338" stopIfTrue="1">
       <formula>AND($C22="Risque élevé",I$5&gt;=$F22,I$5&lt;=$F22+$G22-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="124" priority="339" stopIfTrue="1">
+    <cfRule type="expression" dxfId="127" priority="339" stopIfTrue="1">
       <formula>AND($C22="En bonne voie",I$5&gt;=$F22,I$5&lt;=$F22+$G22-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="123" priority="340" stopIfTrue="1">
+    <cfRule type="expression" dxfId="126" priority="340" stopIfTrue="1">
       <formula>AND($C22="Risque moyen",I$5&gt;=$F22,I$5&lt;=$F22+$G22-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="122" priority="341" stopIfTrue="1">
+    <cfRule type="expression" dxfId="125" priority="341" stopIfTrue="1">
       <formula>AND(LEN($C22)=0,I$5&gt;=$F22,I$5&lt;=$F22+$G22-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB22">
-    <cfRule type="expression" dxfId="121" priority="342">
+    <cfRule type="expression" dxfId="124" priority="342">
       <formula>AND(TODAY()&gt;=AB$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10822,29 +10833,29 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I20:AA20">
-    <cfRule type="expression" dxfId="120" priority="326">
+    <cfRule type="expression" dxfId="123" priority="326">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I20:AB20">
-    <cfRule type="expression" dxfId="119" priority="328" stopIfTrue="1">
+    <cfRule type="expression" dxfId="122" priority="328" stopIfTrue="1">
       <formula>AND($C20="Risque faible",I$5&gt;=$F20,I$5&lt;=$F20+$G20-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="118" priority="329" stopIfTrue="1">
+    <cfRule type="expression" dxfId="121" priority="329" stopIfTrue="1">
       <formula>AND($C20="Risque élevé",I$5&gt;=$F20,I$5&lt;=$F20+$G20-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="117" priority="330" stopIfTrue="1">
+    <cfRule type="expression" dxfId="120" priority="330" stopIfTrue="1">
       <formula>AND($C20="En bonne voie",I$5&gt;=$F20,I$5&lt;=$F20+$G20-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="116" priority="331" stopIfTrue="1">
+    <cfRule type="expression" dxfId="119" priority="331" stopIfTrue="1">
       <formula>AND($C20="Risque moyen",I$5&gt;=$F20,I$5&lt;=$F20+$G20-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="115" priority="332" stopIfTrue="1">
+    <cfRule type="expression" dxfId="118" priority="332" stopIfTrue="1">
       <formula>AND(LEN($C20)=0,I$5&gt;=$F20,I$5&lt;=$F20+$G20-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB20">
-    <cfRule type="expression" dxfId="114" priority="333">
+    <cfRule type="expression" dxfId="117" priority="333">
       <formula>AND(TODAY()&gt;=AB$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10863,7 +10874,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I40:AA41">
-    <cfRule type="expression" dxfId="113" priority="263">
+    <cfRule type="expression" dxfId="116" priority="263">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10882,29 +10893,29 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I43:AA43">
-    <cfRule type="expression" dxfId="112" priority="290">
+    <cfRule type="expression" dxfId="115" priority="290">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I43:AB43">
-    <cfRule type="expression" dxfId="111" priority="292" stopIfTrue="1">
+    <cfRule type="expression" dxfId="114" priority="292" stopIfTrue="1">
       <formula>AND($C43="Risque faible",I$5&gt;=$F43,I$5&lt;=$F43+$G43-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="110" priority="293" stopIfTrue="1">
+    <cfRule type="expression" dxfId="113" priority="293" stopIfTrue="1">
       <formula>AND($C43="Risque élevé",I$5&gt;=$F43,I$5&lt;=$F43+$G43-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="109" priority="294" stopIfTrue="1">
+    <cfRule type="expression" dxfId="112" priority="294" stopIfTrue="1">
       <formula>AND($C43="En bonne voie",I$5&gt;=$F43,I$5&lt;=$F43+$G43-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="108" priority="295" stopIfTrue="1">
+    <cfRule type="expression" dxfId="111" priority="295" stopIfTrue="1">
       <formula>AND($C43="Risque moyen",I$5&gt;=$F43,I$5&lt;=$F43+$G43-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="107" priority="296" stopIfTrue="1">
+    <cfRule type="expression" dxfId="110" priority="296" stopIfTrue="1">
       <formula>AND(LEN($C43)=0,I$5&gt;=$F43,I$5&lt;=$F43+$G43-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB43">
-    <cfRule type="expression" dxfId="106" priority="297">
+    <cfRule type="expression" dxfId="109" priority="297">
       <formula>AND(TODAY()&gt;=AB$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10923,51 +10934,51 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I36:AA37">
-    <cfRule type="expression" dxfId="105" priority="281">
+    <cfRule type="expression" dxfId="108" priority="281">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I36:AB37">
-    <cfRule type="expression" dxfId="104" priority="283" stopIfTrue="1">
+    <cfRule type="expression" dxfId="107" priority="283" stopIfTrue="1">
       <formula>AND($C36="Risque faible",I$5&gt;=$F36,I$5&lt;=$F36+$G36-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="103" priority="284" stopIfTrue="1">
+    <cfRule type="expression" dxfId="106" priority="284" stopIfTrue="1">
       <formula>AND($C36="Risque élevé",I$5&gt;=$F36,I$5&lt;=$F36+$G36-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="102" priority="285" stopIfTrue="1">
+    <cfRule type="expression" dxfId="105" priority="285" stopIfTrue="1">
       <formula>AND($C36="En bonne voie",I$5&gt;=$F36,I$5&lt;=$F36+$G36-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="101" priority="286" stopIfTrue="1">
+    <cfRule type="expression" dxfId="104" priority="286" stopIfTrue="1">
       <formula>AND($C36="Risque moyen",I$5&gt;=$F36,I$5&lt;=$F36+$G36-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="100" priority="287" stopIfTrue="1">
+    <cfRule type="expression" dxfId="103" priority="287" stopIfTrue="1">
       <formula>AND(LEN($C36)=0,I$5&gt;=$F36,I$5&lt;=$F36+$G36-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB36:AB37">
-    <cfRule type="expression" dxfId="99" priority="288">
+    <cfRule type="expression" dxfId="102" priority="288">
       <formula>AND(TODAY()&gt;=AB$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I40:AB41">
-    <cfRule type="expression" dxfId="98" priority="265" stopIfTrue="1">
+    <cfRule type="expression" dxfId="101" priority="265" stopIfTrue="1">
       <formula>AND($C40="Risque faible",I$5&gt;=$F40,I$5&lt;=$F40+$G40-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="97" priority="266" stopIfTrue="1">
+    <cfRule type="expression" dxfId="100" priority="266" stopIfTrue="1">
       <formula>AND($C40="Risque élevé",I$5&gt;=$F40,I$5&lt;=$F40+$G40-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="96" priority="267" stopIfTrue="1">
+    <cfRule type="expression" dxfId="99" priority="267" stopIfTrue="1">
       <formula>AND($C40="En bonne voie",I$5&gt;=$F40,I$5&lt;=$F40+$G40-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="95" priority="268" stopIfTrue="1">
+    <cfRule type="expression" dxfId="98" priority="268" stopIfTrue="1">
       <formula>AND($C40="Risque moyen",I$5&gt;=$F40,I$5&lt;=$F40+$G40-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="94" priority="269" stopIfTrue="1">
+    <cfRule type="expression" dxfId="97" priority="269" stopIfTrue="1">
       <formula>AND(LEN($C40)=0,I$5&gt;=$F40,I$5&lt;=$F40+$G40-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB40:AB41">
-    <cfRule type="expression" dxfId="93" priority="270">
+    <cfRule type="expression" dxfId="96" priority="270">
       <formula>AND(TODAY()&gt;=AB$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10986,56 +10997,56 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I45:AA47">
-    <cfRule type="expression" dxfId="92" priority="254">
+    <cfRule type="expression" dxfId="95" priority="254">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I45:AB47">
-    <cfRule type="expression" dxfId="91" priority="256" stopIfTrue="1">
+    <cfRule type="expression" dxfId="94" priority="256" stopIfTrue="1">
       <formula>AND($C45="Risque faible",I$5&gt;=$F45,I$5&lt;=$F45+$G45-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="90" priority="257" stopIfTrue="1">
+    <cfRule type="expression" dxfId="93" priority="257" stopIfTrue="1">
       <formula>AND($C45="Risque élevé",I$5&gt;=$F45,I$5&lt;=$F45+$G45-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="89" priority="258" stopIfTrue="1">
+    <cfRule type="expression" dxfId="92" priority="258" stopIfTrue="1">
       <formula>AND($C45="En bonne voie",I$5&gt;=$F45,I$5&lt;=$F45+$G45-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="88" priority="259" stopIfTrue="1">
+    <cfRule type="expression" dxfId="91" priority="259" stopIfTrue="1">
       <formula>AND($C45="Risque moyen",I$5&gt;=$F45,I$5&lt;=$F45+$G45-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="87" priority="260" stopIfTrue="1">
+    <cfRule type="expression" dxfId="90" priority="260" stopIfTrue="1">
       <formula>AND(LEN($C45)=0,I$5&gt;=$F45,I$5&lt;=$F45+$G45-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB45:AB47">
-    <cfRule type="expression" dxfId="86" priority="261">
+    <cfRule type="expression" dxfId="89" priority="261">
       <formula>AND(TODAY()&gt;=AB$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I35:AB35">
-    <cfRule type="expression" dxfId="85" priority="240" stopIfTrue="1">
+    <cfRule type="expression" dxfId="88" priority="240" stopIfTrue="1">
       <formula>AND($C35="Risque faible",I$5&gt;=$F35,I$5&lt;=$F35+$G35-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="84" priority="241" stopIfTrue="1">
+    <cfRule type="expression" dxfId="87" priority="241" stopIfTrue="1">
       <formula>AND($C35="Risque élevé",I$5&gt;=$F35,I$5&lt;=$F35+$G35-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="83" priority="242" stopIfTrue="1">
+    <cfRule type="expression" dxfId="86" priority="242" stopIfTrue="1">
       <formula>AND($C35="En bonne voie",I$5&gt;=$F35,I$5&lt;=$F35+$G35-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="82" priority="243" stopIfTrue="1">
+    <cfRule type="expression" dxfId="85" priority="243" stopIfTrue="1">
       <formula>AND($C35="Risque moyen",I$5&gt;=$F35,I$5&lt;=$F35+$G35-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="81" priority="244" stopIfTrue="1">
+    <cfRule type="expression" dxfId="84" priority="244" stopIfTrue="1">
       <formula>AND(LEN($C35)=0,I$5&gt;=$F35,I$5&lt;=$F35+$G35-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I35:AA35">
-    <cfRule type="expression" dxfId="80" priority="237">
+    <cfRule type="expression" dxfId="83" priority="237">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB35">
-    <cfRule type="expression" dxfId="79" priority="238">
+    <cfRule type="expression" dxfId="82" priority="238">
       <formula>AND(TODAY()&gt;=AB$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11068,29 +11079,29 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I38:AA38">
-    <cfRule type="expression" dxfId="78" priority="227">
+    <cfRule type="expression" dxfId="81" priority="227">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I38:AB38">
-    <cfRule type="expression" dxfId="77" priority="229" stopIfTrue="1">
+    <cfRule type="expression" dxfId="80" priority="229" stopIfTrue="1">
       <formula>AND($C38="Risque faible",I$5&gt;=$F38,I$5&lt;=$F38+$G38-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="76" priority="230" stopIfTrue="1">
+    <cfRule type="expression" dxfId="79" priority="230" stopIfTrue="1">
       <formula>AND($C38="Risque élevé",I$5&gt;=$F38,I$5&lt;=$F38+$G38-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="75" priority="231" stopIfTrue="1">
+    <cfRule type="expression" dxfId="78" priority="231" stopIfTrue="1">
       <formula>AND($C38="En bonne voie",I$5&gt;=$F38,I$5&lt;=$F38+$G38-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="74" priority="232" stopIfTrue="1">
+    <cfRule type="expression" dxfId="77" priority="232" stopIfTrue="1">
       <formula>AND($C38="Risque moyen",I$5&gt;=$F38,I$5&lt;=$F38+$G38-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="73" priority="233" stopIfTrue="1">
+    <cfRule type="expression" dxfId="76" priority="233" stopIfTrue="1">
       <formula>AND(LEN($C38)=0,I$5&gt;=$F38,I$5&lt;=$F38+$G38-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB38">
-    <cfRule type="expression" dxfId="72" priority="234">
+    <cfRule type="expression" dxfId="75" priority="234">
       <formula>AND(TODAY()&gt;=AB$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11109,29 +11120,29 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I48:AA49">
-    <cfRule type="expression" dxfId="71" priority="209">
+    <cfRule type="expression" dxfId="74" priority="209">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I48:AB49">
-    <cfRule type="expression" dxfId="70" priority="211" stopIfTrue="1">
+    <cfRule type="expression" dxfId="73" priority="211" stopIfTrue="1">
       <formula>AND($C48="Risque faible",I$5&gt;=$F48,I$5&lt;=$F48+$G48-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="69" priority="212" stopIfTrue="1">
+    <cfRule type="expression" dxfId="72" priority="212" stopIfTrue="1">
       <formula>AND($C48="Risque élevé",I$5&gt;=$F48,I$5&lt;=$F48+$G48-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="68" priority="213" stopIfTrue="1">
+    <cfRule type="expression" dxfId="71" priority="213" stopIfTrue="1">
       <formula>AND($C48="En bonne voie",I$5&gt;=$F48,I$5&lt;=$F48+$G48-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="67" priority="214" stopIfTrue="1">
+    <cfRule type="expression" dxfId="70" priority="214" stopIfTrue="1">
       <formula>AND($C48="Risque moyen",I$5&gt;=$F48,I$5&lt;=$F48+$G48-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="66" priority="215" stopIfTrue="1">
+    <cfRule type="expression" dxfId="69" priority="215" stopIfTrue="1">
       <formula>AND(LEN($C48)=0,I$5&gt;=$F48,I$5&lt;=$F48+$G48-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB48:AB49">
-    <cfRule type="expression" dxfId="65" priority="216">
+    <cfRule type="expression" dxfId="68" priority="216">
       <formula>AND(TODAY()&gt;=AB$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11150,29 +11161,29 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I52:AA53">
-    <cfRule type="expression" dxfId="64" priority="200">
+    <cfRule type="expression" dxfId="67" priority="200">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I52:AB53">
-    <cfRule type="expression" dxfId="63" priority="202" stopIfTrue="1">
+    <cfRule type="expression" dxfId="66" priority="202" stopIfTrue="1">
       <formula>AND($C52="Risque faible",I$5&gt;=$F52,I$5&lt;=$F52+$G52-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="62" priority="203" stopIfTrue="1">
+    <cfRule type="expression" dxfId="65" priority="203" stopIfTrue="1">
       <formula>AND($C52="Risque élevé",I$5&gt;=$F52,I$5&lt;=$F52+$G52-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="61" priority="204" stopIfTrue="1">
+    <cfRule type="expression" dxfId="64" priority="204" stopIfTrue="1">
       <formula>AND($C52="En bonne voie",I$5&gt;=$F52,I$5&lt;=$F52+$G52-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="60" priority="205" stopIfTrue="1">
+    <cfRule type="expression" dxfId="63" priority="205" stopIfTrue="1">
       <formula>AND($C52="Risque moyen",I$5&gt;=$F52,I$5&lt;=$F52+$G52-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="59" priority="206" stopIfTrue="1">
+    <cfRule type="expression" dxfId="62" priority="206" stopIfTrue="1">
       <formula>AND(LEN($C52)=0,I$5&gt;=$F52,I$5&lt;=$F52+$G52-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB52:AB53">
-    <cfRule type="expression" dxfId="58" priority="207">
+    <cfRule type="expression" dxfId="61" priority="207">
       <formula>AND(TODAY()&gt;=AB$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11191,7 +11202,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I55:AA55">
-    <cfRule type="expression" dxfId="57" priority="145">
+    <cfRule type="expression" dxfId="60" priority="145">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11210,61 +11221,61 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I56:AA56">
-    <cfRule type="expression" dxfId="56" priority="154">
+    <cfRule type="expression" dxfId="59" priority="154">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB56">
-    <cfRule type="expression" dxfId="55" priority="161">
+    <cfRule type="expression" dxfId="58" priority="161">
       <formula>AND(TODAY()&gt;=AB$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I55:AB55">
-    <cfRule type="expression" dxfId="54" priority="149" stopIfTrue="1">
+    <cfRule type="expression" dxfId="57" priority="149" stopIfTrue="1">
       <formula>AND($C55="Risque faible",I$5&gt;=$F55,I$5&lt;=$F55+$G55-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="53" priority="150" stopIfTrue="1">
+    <cfRule type="expression" dxfId="56" priority="150" stopIfTrue="1">
       <formula>AND($C55="Risque élevé",I$5&gt;=$F55,I$5&lt;=$F55+$G55-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="52" priority="151" stopIfTrue="1">
+    <cfRule type="expression" dxfId="55" priority="151" stopIfTrue="1">
       <formula>AND($C55="En bonne voie",I$5&gt;=$F55,I$5&lt;=$F55+$G55-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="51" priority="152" stopIfTrue="1">
+    <cfRule type="expression" dxfId="54" priority="152" stopIfTrue="1">
       <formula>AND($C55="Risque moyen",I$5&gt;=$F55,I$5&lt;=$F55+$G55-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="50" priority="153" stopIfTrue="1">
+    <cfRule type="expression" dxfId="53" priority="153" stopIfTrue="1">
       <formula>AND(LEN($C55)=0,I$5&gt;=$F55,I$5&lt;=$F55+$G55-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB55">
-    <cfRule type="expression" dxfId="49" priority="147">
+    <cfRule type="expression" dxfId="52" priority="147">
       <formula>AND(TODAY()&gt;=AB$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB58">
-    <cfRule type="expression" dxfId="48" priority="93">
+    <cfRule type="expression" dxfId="51" priority="93">
       <formula>AND(TODAY()&gt;=AB$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I58:AB58">
-    <cfRule type="expression" dxfId="47" priority="95" stopIfTrue="1">
+    <cfRule type="expression" dxfId="50" priority="95" stopIfTrue="1">
       <formula>AND($C58="Risque faible",I$5&gt;=$F58,I$5&lt;=$F58+$G58-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="46" priority="96" stopIfTrue="1">
+    <cfRule type="expression" dxfId="49" priority="96" stopIfTrue="1">
       <formula>AND($C58="Risque élevé",I$5&gt;=$F58,I$5&lt;=$F58+$G58-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="45" priority="97" stopIfTrue="1">
+    <cfRule type="expression" dxfId="48" priority="97" stopIfTrue="1">
       <formula>AND($C58="En bonne voie",I$5&gt;=$F58,I$5&lt;=$F58+$G58-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="44" priority="98" stopIfTrue="1">
+    <cfRule type="expression" dxfId="47" priority="98" stopIfTrue="1">
       <formula>AND($C58="Risque moyen",I$5&gt;=$F58,I$5&lt;=$F58+$G58-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="43" priority="99" stopIfTrue="1">
+    <cfRule type="expression" dxfId="46" priority="99" stopIfTrue="1">
       <formula>AND(LEN($C58)=0,I$5&gt;=$F58,I$5&lt;=$F58+$G58-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I58:AA58">
-    <cfRule type="expression" dxfId="42" priority="92">
+    <cfRule type="expression" dxfId="45" priority="92">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11297,22 +11308,22 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I59:AA60">
-    <cfRule type="expression" dxfId="41" priority="46">
+    <cfRule type="expression" dxfId="44" priority="46">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB59:AB60">
-    <cfRule type="expression" dxfId="40" priority="48">
+    <cfRule type="expression" dxfId="43" priority="48">
       <formula>AND(TODAY()&gt;=AB$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I62:AA62">
-    <cfRule type="expression" dxfId="39" priority="29">
+    <cfRule type="expression" dxfId="42" priority="29">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB61">
-    <cfRule type="expression" dxfId="38" priority="39">
+    <cfRule type="expression" dxfId="41" priority="39">
       <formula>AND(TODAY()&gt;=AB$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11345,80 +11356,80 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I61:AA61">
-    <cfRule type="expression" dxfId="37" priority="37">
+    <cfRule type="expression" dxfId="40" priority="37">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I59:AB60">
-    <cfRule type="expression" dxfId="36" priority="50" stopIfTrue="1">
+    <cfRule type="expression" dxfId="39" priority="50" stopIfTrue="1">
       <formula>AND($C59="Risque faible",I$5&gt;=$F59,I$5&lt;=$F59+$G59-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="35" priority="51" stopIfTrue="1">
+    <cfRule type="expression" dxfId="38" priority="51" stopIfTrue="1">
       <formula>AND($C59="Risque élevé",I$5&gt;=$F59,I$5&lt;=$F59+$G59-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="52" stopIfTrue="1">
+    <cfRule type="expression" dxfId="37" priority="52" stopIfTrue="1">
       <formula>AND($C59="En bonne voie",I$5&gt;=$F59,I$5&lt;=$F59+$G59-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="53" stopIfTrue="1">
+    <cfRule type="expression" dxfId="36" priority="53" stopIfTrue="1">
       <formula>AND($C59="Risque moyen",I$5&gt;=$F59,I$5&lt;=$F59+$G59-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="54" stopIfTrue="1">
+    <cfRule type="expression" dxfId="35" priority="54" stopIfTrue="1">
       <formula>AND(LEN($C59)=0,I$5&gt;=$F59,I$5&lt;=$F59+$G59-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I61:AB61">
-    <cfRule type="expression" dxfId="31" priority="41" stopIfTrue="1">
+    <cfRule type="expression" dxfId="34" priority="41" stopIfTrue="1">
       <formula>AND($C61="Risque faible",I$5&gt;=$F61,I$5&lt;=$F61+$G61-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="42" stopIfTrue="1">
+    <cfRule type="expression" dxfId="33" priority="42" stopIfTrue="1">
       <formula>AND($C61="Risque élevé",I$5&gt;=$F61,I$5&lt;=$F61+$G61-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="43" stopIfTrue="1">
+    <cfRule type="expression" dxfId="32" priority="43" stopIfTrue="1">
       <formula>AND($C61="En bonne voie",I$5&gt;=$F61,I$5&lt;=$F61+$G61-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="44" stopIfTrue="1">
+    <cfRule type="expression" dxfId="31" priority="44" stopIfTrue="1">
       <formula>AND($C61="Risque moyen",I$5&gt;=$F61,I$5&lt;=$F61+$G61-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="45" stopIfTrue="1">
+    <cfRule type="expression" dxfId="30" priority="45" stopIfTrue="1">
       <formula>AND(LEN($C61)=0,I$5&gt;=$F61,I$5&lt;=$F61+$G61-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB62">
-    <cfRule type="expression" dxfId="26" priority="30">
+    <cfRule type="expression" dxfId="29" priority="30">
       <formula>AND(TODAY()&gt;=AB$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I62:AB62">
-    <cfRule type="expression" dxfId="25" priority="32" stopIfTrue="1">
+    <cfRule type="expression" dxfId="28" priority="32" stopIfTrue="1">
       <formula>AND($C62="Risque faible",I$5&gt;=$F62,I$5&lt;=$F62+$G62-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="33" stopIfTrue="1">
+    <cfRule type="expression" dxfId="27" priority="33" stopIfTrue="1">
       <formula>AND($C62="Risque élevé",I$5&gt;=$F62,I$5&lt;=$F62+$G62-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="34" stopIfTrue="1">
+    <cfRule type="expression" dxfId="26" priority="34" stopIfTrue="1">
       <formula>AND($C62="En bonne voie",I$5&gt;=$F62,I$5&lt;=$F62+$G62-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="35" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="35" stopIfTrue="1">
       <formula>AND($C62="Risque moyen",I$5&gt;=$F62,I$5&lt;=$F62+$G62-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="36" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="36" stopIfTrue="1">
       <formula>AND(LEN($C62)=0,I$5&gt;=$F62,I$5&lt;=$F62+$G62-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I63:AB63">
-    <cfRule type="expression" dxfId="20" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="23" stopIfTrue="1">
       <formula>AND($C63="Risque faible",I$5&gt;=$F63,I$5&lt;=$F63+$G63-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="24" stopIfTrue="1">
       <formula>AND($C63="Risque élevé",I$5&gt;=$F63,I$5&lt;=$F63+$G63-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="25" stopIfTrue="1">
       <formula>AND($C63="En bonne voie",I$5&gt;=$F63,I$5&lt;=$F63+$G63-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="20" priority="26" stopIfTrue="1">
       <formula>AND($C63="Risque moyen",I$5&gt;=$F63,I$5&lt;=$F63+$G63-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="27" stopIfTrue="1">
       <formula>AND(LEN($C63)=0,I$5&gt;=$F63,I$5&lt;=$F63+$G63-1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11437,29 +11448,29 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I63:AA63">
-    <cfRule type="expression" dxfId="15" priority="19">
+    <cfRule type="expression" dxfId="18" priority="19">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB63">
-    <cfRule type="expression" dxfId="14" priority="21">
+    <cfRule type="expression" dxfId="17" priority="21">
       <formula>AND(TODAY()&gt;=AB$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I64:AB64">
-    <cfRule type="expression" dxfId="13" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="14" stopIfTrue="1">
       <formula>AND($C64="Risque faible",I$5&gt;=$F64,I$5&lt;=$F64+$G64-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="15" stopIfTrue="1">
       <formula>AND($C64="Risque élevé",I$5&gt;=$F64,I$5&lt;=$F64+$G64-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="16" stopIfTrue="1">
       <formula>AND($C64="En bonne voie",I$5&gt;=$F64,I$5&lt;=$F64+$G64-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="17" stopIfTrue="1">
       <formula>AND($C64="Risque moyen",I$5&gt;=$F64,I$5&lt;=$F64+$G64-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="18" stopIfTrue="1">
       <formula>AND(LEN($C64)=0,I$5&gt;=$F64,I$5&lt;=$F64+$G64-1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11478,17 +11489,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I64:AA64">
-    <cfRule type="expression" dxfId="8" priority="10">
+    <cfRule type="expression" dxfId="11" priority="10">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB64">
-    <cfRule type="expression" dxfId="7" priority="12">
+    <cfRule type="expression" dxfId="10" priority="12">
       <formula>AND(TODAY()&gt;=AB$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I65:AA65">
-    <cfRule type="expression" dxfId="6" priority="2">
+    <cfRule type="expression" dxfId="9" priority="2">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11507,24 +11518,24 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB65">
-    <cfRule type="expression" dxfId="5" priority="3">
+    <cfRule type="expression" dxfId="8" priority="3">
       <formula>AND(TODAY()&gt;=AB$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I65:AB65">
-    <cfRule type="expression" dxfId="4" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="5" stopIfTrue="1">
       <formula>AND($C65="Risque faible",I$5&gt;=$F65,I$5&lt;=$F65+$G65-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="6" stopIfTrue="1">
       <formula>AND($C65="Risque élevé",I$5&gt;=$F65,I$5&lt;=$F65+$G65-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="7" stopIfTrue="1">
       <formula>AND($C65="En bonne voie",I$5&gt;=$F65,I$5&lt;=$F65+$G65-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="8" stopIfTrue="1">
       <formula>AND($C65="Risque moyen",I$5&gt;=$F65,I$5&lt;=$F65+$G65-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="9" stopIfTrue="1">
       <formula>AND(LEN($C65)=0,I$5&gt;=$F65,I$5&lt;=$F65+$G65-1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11774,6 +11785,381 @@
           <xm:sqref>E51</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{B7458B1E-89A7-4035-AAD0-B4EF57EC5395}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>E30</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{C5648DCB-335E-4B0D-A272-6F74C3F9FC93}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>E32</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{55FDD253-E1AD-46E7-B4B2-049EF2039EEC}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>E19</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{088C9F7E-CA69-4E46-AE57-65AB9C1B43F2}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>E34</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{2A646182-6DCD-41D3-B1FC-FD0BD97E7EB4}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>E22</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{07BB0CFE-FBB6-4943-8C1E-48527304A5A5}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>E27:E28</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{897BEF3A-AB81-43B7-A43E-B08908C1AA19}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>E24:E25</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{7FBA420F-936F-4508-A0AD-94C2EC401FB3}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>E20</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{B64FBEBF-B38B-4E23-AAA1-91D0ED618B42}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>E40:E41</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{7ECBC1F5-86CA-42A4-874C-8C94FE680DD8}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>E43</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{4B6A1F15-41AD-46DB-A0E2-CC6291CEB3B9}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>E36:E37</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{E50629AE-4ED2-45DA-B67C-3CEE49679E5F}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>E45:E47</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{60857565-07DD-43B4-A08A-A9316D4E4223}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>E35</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{F397BBBD-F9C4-49C1-9309-39EACB50A4EC}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>E38</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{12C5A9C6-10DB-49E8-9E4B-D2B7F47D4CF9}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>E48:E49</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{C06F97DA-CE73-4EC6-A05B-B1FB73BB5B34}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>E52:E53</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{6D0B9FB5-F9CE-42AC-9D63-CA5848E39A6E}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>E55</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{5956CA58-EF61-4E17-99E7-3B18CA15DB7F}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>E56</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{C0E29D5B-20CB-4D30-948E-E90BE31F636D}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>E58</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{7BA5B507-194D-462E-8E0D-BA9490DDCB82}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>E59:E60</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{EE2A084F-CD4E-443B-9F05-519A4985B074}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>E62</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{55E82E44-C53D-446A-B47E-A546B864BBFA}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>E61</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{FDCCC79C-CD8C-4140-A8D0-A0ED96E46894}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>E63</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{D0DD4C81-866F-4BBC-9627-C8F89D3E1C16}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>E64</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{C019EDF8-0993-4E6F-BBC6-62A4A373AC33}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>E65</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="714" id="{628A03C6-EE71-4B44-A6BA-69DC45906EA6}">
             <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
               <x14:cfvo type="percent">
@@ -12002,21 +12388,6 @@
           <xm:sqref>I51:AB51</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{B7458B1E-89A7-4035-AAD0-B4EF57EC5395}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="num">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>E30</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="479" id="{28E3D5FF-7874-452A-A900-6AEA95466C37}">
             <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
               <x14:cfvo type="percent">
@@ -12036,21 +12407,6 @@
           <xm:sqref>I30:AB30</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{C5648DCB-335E-4B0D-A272-6F74C3F9FC93}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="num">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>E32</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="470" id="{EC388F78-FEFF-4C31-A322-84A70D95C998}">
             <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
               <x14:cfvo type="percent">
@@ -12070,21 +12426,6 @@
           <xm:sqref>I32:AB32</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{55FDD253-E1AD-46E7-B4B2-049EF2039EEC}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="num">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>E19</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="461" id="{771D04B8-E599-4047-9D2C-0D8164B3B415}">
             <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
               <x14:cfvo type="percent">
@@ -12104,21 +12445,6 @@
           <xm:sqref>I19:AB19</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{088C9F7E-CA69-4E46-AE57-65AB9C1B43F2}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="num">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>E34</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="389" id="{86F81114-0858-46FD-89A5-B77B20D08E09}">
             <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
               <x14:cfvo type="percent">
@@ -12138,36 +12464,6 @@
           <xm:sqref>I34:AB34</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{2A646182-6DCD-41D3-B1FC-FD0BD97E7EB4}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="num">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>E22</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{07BB0CFE-FBB6-4943-8C1E-48527304A5A5}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="num">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>E27:E28</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="361" id="{B37227A7-F3EB-494D-BE63-027ED68866C7}">
             <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
               <x14:cfvo type="percent">
@@ -12185,21 +12481,6 @@
             </x14:iconSet>
           </x14:cfRule>
           <xm:sqref>I27:AB28</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{897BEF3A-AB81-43B7-A43E-B08908C1AA19}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="num">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>E24:E25</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="352" id="{11F29DBB-9C3A-40BB-A8C9-DD464C4407DD}">
@@ -12240,21 +12521,6 @@
           <xm:sqref>I22:AB22</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{7FBA420F-936F-4508-A0AD-94C2EC401FB3}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="num">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>E20</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="334" id="{3EB16589-8FA1-40F5-9A1D-03F367216E76}">
             <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
               <x14:cfvo type="percent">
@@ -12274,36 +12540,6 @@
           <xm:sqref>I20:AB20</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{B64FBEBF-B38B-4E23-AAA1-91D0ED618B42}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="num">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>E40:E41</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{7ECBC1F5-86CA-42A4-874C-8C94FE680DD8}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="num">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>E43</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="298" id="{9703D153-F9D2-4539-959D-39C677DE5E46}">
             <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
               <x14:cfvo type="percent">
@@ -12321,21 +12557,6 @@
             </x14:iconSet>
           </x14:cfRule>
           <xm:sqref>I43:AB43</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{4B6A1F15-41AD-46DB-A0E2-CC6291CEB3B9}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="num">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>E36:E37</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="289" id="{3C8C73C2-5882-4D50-A619-E8929324CEEC}">
@@ -12376,21 +12597,6 @@
           <xm:sqref>I40:AB41</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{E50629AE-4ED2-45DA-B67C-3CEE49679E5F}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="num">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>E45:E47</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="262" id="{472C0571-07BE-40E4-9871-D2A65C7AE928}">
             <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
               <x14:cfvo type="percent">
@@ -12410,21 +12616,6 @@
           <xm:sqref>I45:AB47</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{60857565-07DD-43B4-A08A-A9316D4E4223}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="num">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>E35</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="239" id="{3BE21401-6C53-4176-97B2-58F16FBEE64E}">
             <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
               <x14:cfvo type="percent">
@@ -12444,21 +12635,6 @@
           <xm:sqref>I35:AB35</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{F397BBBD-F9C4-49C1-9309-39EACB50A4EC}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="num">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>E38</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="235" id="{5854C059-CE8A-46A8-9DE3-850FF95EEC5D}">
             <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
               <x14:cfvo type="percent">
@@ -12478,21 +12654,6 @@
           <xm:sqref>I38:AB38</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{12C5A9C6-10DB-49E8-9E4B-D2B7F47D4CF9}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="num">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>E48:E49</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="217" id="{35F291B0-AC08-4DEC-AC71-E2527C6395F3}">
             <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
               <x14:cfvo type="percent">
@@ -12510,21 +12671,6 @@
             </x14:iconSet>
           </x14:cfRule>
           <xm:sqref>I48:AB49</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{C06F97DA-CE73-4EC6-A05B-B1FB73BB5B34}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="num">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>E52:E53</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="208" id="{63E239F2-C90C-4923-A631-FDFBBBCB6804}">
@@ -12584,36 +12730,6 @@
           <xm:sqref>I57:AB57</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{6D0B9FB5-F9CE-42AC-9D63-CA5848E39A6E}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="num">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>E55</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{5956CA58-EF61-4E17-99E7-3B18CA15DB7F}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="num">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>E56</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="162" id="{1BF54B70-B0A3-451B-82EE-99FB2164159D}">
             <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
               <x14:cfvo type="percent">
@@ -12652,21 +12768,6 @@
           <xm:sqref>I55:AB55</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{C0E29D5B-20CB-4D30-948E-E90BE31F636D}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="num">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>E58</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="94" id="{19020CA2-A634-4E23-B0F2-6254842B5EB1}">
             <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
               <x14:cfvo type="percent">
@@ -12684,51 +12785,6 @@
             </x14:iconSet>
           </x14:cfRule>
           <xm:sqref>I58:AB58</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{7BA5B507-194D-462E-8E0D-BA9490DDCB82}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="num">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>E59:E60</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{EE2A084F-CD4E-443B-9F05-519A4985B074}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="num">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>E62</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{55E82E44-C53D-446A-B47E-A546B864BBFA}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="num">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>E61</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="49" id="{6235C1BF-8B2E-4174-B0E6-53AF00330DAD}">
@@ -12788,21 +12844,6 @@
           <xm:sqref>I62:AB62</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{FDCCC79C-CD8C-4140-A8D0-A0ED96E46894}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="num">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>E63</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="22" id="{17BED863-7B80-4A47-B388-C01464071AEA}">
             <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
               <x14:cfvo type="percent">
@@ -12822,21 +12863,6 @@
           <xm:sqref>I63:AB63</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{D0DD4C81-866F-4BBC-9627-C8F89D3E1C16}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="num">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>E64</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="13" id="{8987036F-3AE1-4CD0-A7FA-9E6DCDF640DB}">
             <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
               <x14:cfvo type="percent">
@@ -12854,21 +12880,6 @@
             </x14:iconSet>
           </x14:cfRule>
           <xm:sqref>I64:AB64</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{C019EDF8-0993-4E6F-BBC6-62A4A373AC33}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="num">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>E65</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="4" id="{E5E94B63-5356-481B-8A1F-AA218FFD91A9}">
@@ -12901,13 +12912,13 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="87.140625" style="10" customWidth="1"/>
-    <col min="2" max="16384" width="9.140625" style="8"/>
+    <col min="1" max="1" width="87.1640625" style="10" customWidth="1"/>
+    <col min="2" max="16384" width="9.1640625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="9" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:1" s="9" customFormat="1" ht="26" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>24</v>
       </c>
@@ -12922,7 +12933,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:1" s="10" customFormat="1" ht="222" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" s="10" customFormat="1" ht="222" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
         <v>27</v>
       </c>

</xml_diff>

<commit_message>
mise à jour de la plannification
</commit_message>
<xml_diff>
--- a/Diagramme_de_Gantt.xlsx
+++ b/Diagramme_de_Gantt.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{160018D5-DE59-8746-AFCD-303ABBAB6B33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE017EEC-5021-3540-A4A3-9883D7ADA76A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15840" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="89">
   <si>
     <t>Créez un diagramme de Gantt dans cette feuille de calcul.
 Entrez le titre de ce projet dans la cellule B1. 
@@ -6157,8 +6157,8 @@
   </sheetPr>
   <dimension ref="A1:AB68"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A48" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A45" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -7170,7 +7170,7 @@
         <v>50</v>
       </c>
       <c r="E15" s="30">
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="F15" s="51">
         <v>43882</v>
@@ -7266,9 +7266,11 @@
         <v>36</v>
       </c>
       <c r="C16" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="D16" s="33"/>
+        <v>16</v>
+      </c>
+      <c r="D16" s="33" t="s">
+        <v>50</v>
+      </c>
       <c r="E16" s="30">
         <v>0</v>
       </c>
@@ -9981,8 +9983,12 @@
       <c r="B63" s="53" t="s">
         <v>87</v>
       </c>
-      <c r="C63" s="33"/>
-      <c r="D63" s="33"/>
+      <c r="C63" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="D63" s="33" t="s">
+        <v>46</v>
+      </c>
       <c r="E63" s="30">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
ajout dessin garde et petite modification dessin Lode Runner
</commit_message>
<xml_diff>
--- a/Diagramme_de_Gantt.xlsx
+++ b/Diagramme_de_Gantt.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE017EEC-5021-3540-A4A3-9883D7ADA76A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20B26D91-869D-9D4D-943F-32A3125FC1BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15840" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6157,7 +6157,7 @@
   </sheetPr>
   <dimension ref="A1:AB68"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A45" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A20" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
       <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
@@ -7272,7 +7272,7 @@
         <v>50</v>
       </c>
       <c r="E16" s="30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F16" s="51">
         <v>43882</v>
@@ -9764,7 +9764,7 @@
         <v>45</v>
       </c>
       <c r="C57" s="33" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D57" s="33" t="s">
         <v>50</v>
@@ -9984,13 +9984,13 @@
         <v>87</v>
       </c>
       <c r="C63" s="33" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D63" s="33" t="s">
         <v>46</v>
       </c>
       <c r="E63" s="30">
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="F63" s="51">
         <v>43885</v>

</xml_diff>

<commit_message>
déplacement horizontal Lode Runner  et attendre joueur
</commit_message>
<xml_diff>
--- a/Diagramme_de_Gantt.xlsx
+++ b/Diagramme_de_Gantt.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20B26D91-869D-9D4D-943F-32A3125FC1BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91645568-42BF-8F42-A0AE-BDA85DCFCFF7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15840" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28820" yWindow="460" windowWidth="28500" windowHeight="21140" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt" sheetId="11" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="90">
   <si>
     <t>Créez un diagramme de Gantt dans cette feuille de calcul.
 Entrez le titre de ce projet dans la cellule B1. 
@@ -324,6 +324,9 @@
   </si>
   <si>
     <t>Ajouter sons selon situations</t>
+  </si>
+  <si>
+    <t>caroline</t>
   </si>
 </sst>
 </file>
@@ -6157,8 +6160,8 @@
   </sheetPr>
   <dimension ref="A1:AB68"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A20" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="C63" sqref="C63"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -7551,10 +7554,14 @@
       <c r="B19" s="53" t="s">
         <v>54</v>
       </c>
-      <c r="C19" s="33"/>
-      <c r="D19" s="33"/>
+      <c r="C19" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" s="33" t="s">
+        <v>50</v>
+      </c>
       <c r="E19" s="30">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="F19" s="31">
         <v>43886</v>
@@ -7589,7 +7596,9 @@
       <c r="B20" s="53" t="s">
         <v>55</v>
       </c>
-      <c r="C20" s="33"/>
+      <c r="C20" s="33" t="s">
+        <v>15</v>
+      </c>
       <c r="D20" s="33"/>
       <c r="E20" s="30">
         <v>0</v>
@@ -7719,7 +7728,9 @@
       <c r="B22" s="53" t="s">
         <v>56</v>
       </c>
-      <c r="C22" s="33"/>
+      <c r="C22" s="33" t="s">
+        <v>15</v>
+      </c>
       <c r="D22" s="33"/>
       <c r="E22" s="30">
         <v>0</v>
@@ -7849,7 +7860,9 @@
       <c r="B24" s="53" t="s">
         <v>57</v>
       </c>
-      <c r="C24" s="33"/>
+      <c r="C24" s="33" t="s">
+        <v>15</v>
+      </c>
       <c r="D24" s="33"/>
       <c r="E24" s="30">
         <v>0</v>
@@ -7887,7 +7900,9 @@
       <c r="B25" s="53" t="s">
         <v>58</v>
       </c>
-      <c r="C25" s="33"/>
+      <c r="C25" s="33" t="s">
+        <v>15</v>
+      </c>
       <c r="D25" s="33"/>
       <c r="E25" s="30">
         <v>0</v>
@@ -8017,7 +8032,9 @@
       <c r="B27" s="53" t="s">
         <v>60</v>
       </c>
-      <c r="C27" s="33"/>
+      <c r="C27" s="33" t="s">
+        <v>15</v>
+      </c>
       <c r="D27" s="33"/>
       <c r="E27" s="30">
         <v>0</v>
@@ -8055,7 +8072,9 @@
       <c r="B28" s="53" t="s">
         <v>61</v>
       </c>
-      <c r="C28" s="33"/>
+      <c r="C28" s="33" t="s">
+        <v>15</v>
+      </c>
       <c r="D28" s="33"/>
       <c r="E28" s="30">
         <v>0</v>
@@ -8093,7 +8112,9 @@
       <c r="B29" s="50" t="s">
         <v>41</v>
       </c>
-      <c r="C29" s="33"/>
+      <c r="C29" s="33" t="s">
+        <v>15</v>
+      </c>
       <c r="D29" s="33"/>
       <c r="E29" s="30">
         <v>0</v>
@@ -9875,10 +9896,14 @@
       <c r="B60" s="53" t="s">
         <v>84</v>
       </c>
-      <c r="C60" s="33"/>
-      <c r="D60" s="33"/>
+      <c r="C60" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="D60" s="33" t="s">
+        <v>89</v>
+      </c>
       <c r="E60" s="30">
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="F60" s="31">
         <v>43886</v>

</xml_diff>

<commit_message>
mise à jour du calendrier
</commit_message>
<xml_diff>
--- a/Diagramme_de_Gantt.xlsx
+++ b/Diagramme_de_Gantt.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91645568-42BF-8F42-A0AE-BDA85DCFCFF7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EECF8607-7370-E64F-8271-EF1883869D4D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28820" yWindow="460" windowWidth="28500" windowHeight="21140" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16420" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt" sheetId="11" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="90">
   <si>
     <t>Créez un diagramme de Gantt dans cette feuille de calcul.
 Entrez le titre de ce projet dans la cellule B1. 
@@ -326,7 +326,7 @@
     <t>Ajouter sons selon situations</t>
   </si>
   <si>
-    <t>caroline</t>
+    <t>Caroline et Émil</t>
   </si>
 </sst>
 </file>
@@ -6160,8 +6160,8 @@
   </sheetPr>
   <dimension ref="A1:AB68"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -7555,13 +7555,13 @@
         <v>54</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D19" s="33" t="s">
-        <v>50</v>
+        <v>89</v>
       </c>
       <c r="E19" s="30">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="F19" s="31">
         <v>43886</v>
@@ -7597,11 +7597,13 @@
         <v>55</v>
       </c>
       <c r="C20" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="D20" s="33"/>
+        <v>16</v>
+      </c>
+      <c r="D20" s="33" t="s">
+        <v>46</v>
+      </c>
       <c r="E20" s="30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F20" s="31">
         <v>43886</v>
@@ -7729,11 +7731,13 @@
         <v>56</v>
       </c>
       <c r="C22" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="D22" s="33"/>
+        <v>16</v>
+      </c>
+      <c r="D22" s="33" t="s">
+        <v>46</v>
+      </c>
       <c r="E22" s="30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F22" s="31">
         <v>43886</v>
@@ -7861,11 +7865,13 @@
         <v>57</v>
       </c>
       <c r="C24" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="D24" s="33"/>
+        <v>16</v>
+      </c>
+      <c r="D24" s="33" t="s">
+        <v>46</v>
+      </c>
       <c r="E24" s="30">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F24" s="31">
         <v>43888</v>
@@ -8033,11 +8039,13 @@
         <v>60</v>
       </c>
       <c r="C27" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="D27" s="33"/>
+        <v>16</v>
+      </c>
+      <c r="D27" s="33" t="s">
+        <v>46</v>
+      </c>
       <c r="E27" s="30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F27" s="31">
         <v>43887</v>
@@ -8073,11 +8081,13 @@
         <v>61</v>
       </c>
       <c r="C28" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="D28" s="33"/>
+        <v>16</v>
+      </c>
+      <c r="D28" s="33" t="s">
+        <v>46</v>
+      </c>
       <c r="E28" s="30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F28" s="31">
         <v>43887</v>
@@ -8113,11 +8123,13 @@
         <v>41</v>
       </c>
       <c r="C29" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="D29" s="33"/>
+        <v>16</v>
+      </c>
+      <c r="D29" s="33" t="s">
+        <v>46</v>
+      </c>
       <c r="E29" s="30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F29" s="31">
         <v>43888</v>
@@ -8472,10 +8484,14 @@
       <c r="B34" s="50" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="33"/>
-      <c r="D34" s="33"/>
+      <c r="C34" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="D34" s="33" t="s">
+        <v>89</v>
+      </c>
       <c r="E34" s="30">
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="F34" s="31">
         <v>43892</v>
@@ -9480,10 +9496,14 @@
       <c r="B52" s="53" t="s">
         <v>77</v>
       </c>
-      <c r="C52" s="33"/>
-      <c r="D52" s="33"/>
+      <c r="C52" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="D52" s="33" t="s">
+        <v>46</v>
+      </c>
       <c r="E52" s="30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F52" s="31">
         <v>43896</v>
@@ -9578,10 +9598,14 @@
       <c r="B53" s="53" t="s">
         <v>78</v>
       </c>
-      <c r="C53" s="33"/>
-      <c r="D53" s="33"/>
+      <c r="C53" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="D53" s="33" t="s">
+        <v>46</v>
+      </c>
       <c r="E53" s="30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F53" s="31">
         <v>43894</v>
@@ -9746,7 +9770,9 @@
       <c r="B56" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="C56" s="33"/>
+      <c r="C56" s="33" t="s">
+        <v>14</v>
+      </c>
       <c r="D56" s="33"/>
       <c r="E56" s="30">
         <v>0</v>
@@ -9785,13 +9811,13 @@
         <v>45</v>
       </c>
       <c r="C57" s="33" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D57" s="33" t="s">
         <v>50</v>
       </c>
       <c r="E57" s="30">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="F57" s="51">
         <v>43882</v>
@@ -9858,10 +9884,14 @@
       <c r="B59" s="53" t="s">
         <v>83</v>
       </c>
-      <c r="C59" s="33"/>
-      <c r="D59" s="33"/>
+      <c r="C59" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="D59" s="33" t="s">
+        <v>46</v>
+      </c>
       <c r="E59" s="30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F59" s="31">
         <v>43897</v>
@@ -9897,13 +9927,13 @@
         <v>84</v>
       </c>
       <c r="C60" s="33" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D60" s="33" t="s">
         <v>89</v>
       </c>
       <c r="E60" s="30">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="F60" s="31">
         <v>43886</v>
@@ -10009,13 +10039,13 @@
         <v>87</v>
       </c>
       <c r="C63" s="33" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D63" s="33" t="s">
         <v>46</v>
       </c>
       <c r="E63" s="30">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="F63" s="51">
         <v>43885</v>
@@ -10050,10 +10080,14 @@
       <c r="B64" s="53" t="s">
         <v>88</v>
       </c>
-      <c r="C64" s="33"/>
-      <c r="D64" s="33"/>
+      <c r="C64" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="D64" s="33" t="s">
+        <v>46</v>
+      </c>
       <c r="E64" s="30">
-        <v>0</v>
+        <v>0.35</v>
       </c>
       <c r="F64" s="31">
         <v>43894</v>

</xml_diff>

<commit_message>
modification mouvements LR (amélioration) , MAJ planification, diminution légère de la vitesse de LR
</commit_message>
<xml_diff>
--- a/Diagramme_de_Gantt.xlsx
+++ b/Diagramme_de_Gantt.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1ADA830-82B2-FB46-A647-20D7D37A553B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67153CC9-9E1E-BD4A-B685-8F0F2BA4F06D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28800" yWindow="460" windowWidth="38400" windowHeight="21140" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="94">
   <si>
     <t>Créez un diagramme de Gantt dans cette feuille de calcul.
 Entrez le titre de ce projet dans la cellule B1. 
@@ -1370,6 +1370,15 @@
   </cellStyles>
   <dxfs count="128">
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -3429,15 +3438,6 @@
         <vertical/>
         <horizontal/>
       </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <border>
@@ -3701,9 +3701,9 @@
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Description du jalon" dataDxfId="115"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Catégorie" dataDxfId="114"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Affecté à" dataDxfId="113"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Description du jalon" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Catégorie" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Affecté à" dataDxfId="0"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Avancement"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Début" dataCellStyle="Date"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Nombre de jours"/>
@@ -3985,8 +3985,8 @@
   </sheetPr>
   <dimension ref="A1:AB71"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A37" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="M50" sqref="M50"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A38" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6798,11 +6798,13 @@
         <v>66</v>
       </c>
       <c r="C43" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="D43" s="33"/>
+        <v>15</v>
+      </c>
+      <c r="D43" s="33" t="s">
+        <v>46</v>
+      </c>
       <c r="E43" s="30">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="F43" s="31">
         <v>43894</v>
@@ -7146,11 +7148,13 @@
         <v>71</v>
       </c>
       <c r="C49" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="D49" s="33"/>
+        <v>16</v>
+      </c>
+      <c r="D49" s="33" t="s">
+        <v>46</v>
+      </c>
       <c r="E49" s="30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F49" s="31">
         <v>43896</v>
@@ -7728,11 +7732,13 @@
         <v>79</v>
       </c>
       <c r="C58" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="D58" s="33"/>
+        <v>14</v>
+      </c>
+      <c r="D58" s="33" t="s">
+        <v>90</v>
+      </c>
       <c r="E58" s="30">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="F58" s="31">
         <v>43894</v>
@@ -8216,44 +8222,44 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5:AA13 I16:AA16 I18:AA18 I32:AA32 I21:AA21 I23:AA23 I69:AA69">
-    <cfRule type="expression" dxfId="112" priority="685">
+    <cfRule type="expression" dxfId="115" priority="685">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4:AB4">
-    <cfRule type="expression" dxfId="111" priority="691">
+    <cfRule type="expression" dxfId="114" priority="691">
       <formula>I$5&lt;=EOMONTH($I$5,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:AB4">
-    <cfRule type="expression" dxfId="110" priority="687">
+    <cfRule type="expression" dxfId="113" priority="687">
       <formula>AND(J$5&lt;=EOMONTH($I$5,2),J$5&gt;EOMONTH($I$5,0),J$5&gt;EOMONTH($I$5,1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4:AB4">
-    <cfRule type="expression" dxfId="109" priority="686">
+    <cfRule type="expression" dxfId="112" priority="686">
       <formula>AND(I$5&lt;=EOMONTH($I$5,1),I$5&gt;EOMONTH($I$5,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8:AB13 I16:AB16 I22:AB22 I18:AB20 I58:AB68 I24:AB43 I45:AB56">
-    <cfRule type="expression" dxfId="108" priority="708" stopIfTrue="1">
+    <cfRule type="expression" dxfId="111" priority="708" stopIfTrue="1">
       <formula>AND($C8="Risque faible",I$5&gt;=$F8,I$5&lt;=$F8+$G8-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="107" priority="727" stopIfTrue="1">
+    <cfRule type="expression" dxfId="110" priority="727" stopIfTrue="1">
       <formula>AND($C8="Risque élevé",I$5&gt;=$F8,I$5&lt;=$F8+$G8-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="106" priority="745" stopIfTrue="1">
+    <cfRule type="expression" dxfId="109" priority="745" stopIfTrue="1">
       <formula>AND($C8="En bonne voie",I$5&gt;=$F8,I$5&lt;=$F8+$G8-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="105" priority="746" stopIfTrue="1">
+    <cfRule type="expression" dxfId="108" priority="746" stopIfTrue="1">
       <formula>AND($C8="Risque moyen",I$5&gt;=$F8,I$5&lt;=$F8+$G8-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="104" priority="747" stopIfTrue="1">
+    <cfRule type="expression" dxfId="107" priority="747" stopIfTrue="1">
       <formula>AND(LEN($C8)=0,I$5&gt;=$F8,I$5&lt;=$F8+$G8-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB5:AB13 AB16 AB18 AB32 AB21 AB23 AB69">
-    <cfRule type="expression" dxfId="103" priority="756">
+    <cfRule type="expression" dxfId="106" priority="756">
       <formula>AND(TODAY()&gt;=AB$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8286,29 +8292,29 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I14:AA14">
-    <cfRule type="expression" dxfId="102" priority="667">
+    <cfRule type="expression" dxfId="105" priority="667">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I14:AB14">
-    <cfRule type="expression" dxfId="101" priority="669" stopIfTrue="1">
+    <cfRule type="expression" dxfId="104" priority="669" stopIfTrue="1">
       <formula>AND($C14="Risque faible",I$5&gt;=$F14,I$5&lt;=$F14+$G14-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="100" priority="670" stopIfTrue="1">
+    <cfRule type="expression" dxfId="103" priority="670" stopIfTrue="1">
       <formula>AND($C14="Risque élevé",I$5&gt;=$F14,I$5&lt;=$F14+$G14-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="99" priority="671" stopIfTrue="1">
+    <cfRule type="expression" dxfId="102" priority="671" stopIfTrue="1">
       <formula>AND($C14="En bonne voie",I$5&gt;=$F14,I$5&lt;=$F14+$G14-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="98" priority="672" stopIfTrue="1">
+    <cfRule type="expression" dxfId="101" priority="672" stopIfTrue="1">
       <formula>AND($C14="Risque moyen",I$5&gt;=$F14,I$5&lt;=$F14+$G14-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="97" priority="673" stopIfTrue="1">
+    <cfRule type="expression" dxfId="100" priority="673" stopIfTrue="1">
       <formula>AND(LEN($C14)=0,I$5&gt;=$F14,I$5&lt;=$F14+$G14-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB14">
-    <cfRule type="expression" dxfId="96" priority="674">
+    <cfRule type="expression" dxfId="99" priority="674">
       <formula>AND(TODAY()&gt;=AB$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8327,29 +8333,29 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I15:AA15">
-    <cfRule type="expression" dxfId="95" priority="658">
+    <cfRule type="expression" dxfId="98" priority="658">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I15:AB15">
-    <cfRule type="expression" dxfId="94" priority="660" stopIfTrue="1">
+    <cfRule type="expression" dxfId="97" priority="660" stopIfTrue="1">
       <formula>AND($C15="Risque faible",I$5&gt;=$F15,I$5&lt;=$F15+$G15-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="93" priority="661" stopIfTrue="1">
+    <cfRule type="expression" dxfId="96" priority="661" stopIfTrue="1">
       <formula>AND($C15="Risque élevé",I$5&gt;=$F15,I$5&lt;=$F15+$G15-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="92" priority="662" stopIfTrue="1">
+    <cfRule type="expression" dxfId="95" priority="662" stopIfTrue="1">
       <formula>AND($C15="En bonne voie",I$5&gt;=$F15,I$5&lt;=$F15+$G15-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="91" priority="663" stopIfTrue="1">
+    <cfRule type="expression" dxfId="94" priority="663" stopIfTrue="1">
       <formula>AND($C15="Risque moyen",I$5&gt;=$F15,I$5&lt;=$F15+$G15-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="90" priority="664" stopIfTrue="1">
+    <cfRule type="expression" dxfId="93" priority="664" stopIfTrue="1">
       <formula>AND(LEN($C15)=0,I$5&gt;=$F15,I$5&lt;=$F15+$G15-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB15">
-    <cfRule type="expression" dxfId="89" priority="665">
+    <cfRule type="expression" dxfId="92" priority="665">
       <formula>AND(TODAY()&gt;=AB$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8368,29 +8374,29 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I17:AA17">
-    <cfRule type="expression" dxfId="88" priority="649">
+    <cfRule type="expression" dxfId="91" priority="649">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I17:AB17">
-    <cfRule type="expression" dxfId="87" priority="651" stopIfTrue="1">
+    <cfRule type="expression" dxfId="90" priority="651" stopIfTrue="1">
       <formula>AND($C17="Risque faible",I$5&gt;=$F17,I$5&lt;=$F17+$G17-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="86" priority="652" stopIfTrue="1">
+    <cfRule type="expression" dxfId="89" priority="652" stopIfTrue="1">
       <formula>AND($C17="Risque élevé",I$5&gt;=$F17,I$5&lt;=$F17+$G17-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="85" priority="653" stopIfTrue="1">
+    <cfRule type="expression" dxfId="88" priority="653" stopIfTrue="1">
       <formula>AND($C17="En bonne voie",I$5&gt;=$F17,I$5&lt;=$F17+$G17-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="84" priority="654" stopIfTrue="1">
+    <cfRule type="expression" dxfId="87" priority="654" stopIfTrue="1">
       <formula>AND($C17="Risque moyen",I$5&gt;=$F17,I$5&lt;=$F17+$G17-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="83" priority="655" stopIfTrue="1">
+    <cfRule type="expression" dxfId="86" priority="655" stopIfTrue="1">
       <formula>AND(LEN($C17)=0,I$5&gt;=$F17,I$5&lt;=$F17+$G17-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB17">
-    <cfRule type="expression" dxfId="82" priority="656">
+    <cfRule type="expression" dxfId="85" priority="656">
       <formula>AND(TODAY()&gt;=AB$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8409,12 +8415,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I27:AA27">
-    <cfRule type="expression" dxfId="81" priority="640">
+    <cfRule type="expression" dxfId="84" priority="640">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB27">
-    <cfRule type="expression" dxfId="80" priority="647">
+    <cfRule type="expression" dxfId="83" priority="647">
       <formula>AND(TODAY()&gt;=AB$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8433,12 +8439,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I30:AA30">
-    <cfRule type="expression" dxfId="79" priority="631">
+    <cfRule type="expression" dxfId="82" priority="631">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB30">
-    <cfRule type="expression" dxfId="78" priority="638">
+    <cfRule type="expression" dxfId="81" priority="638">
       <formula>AND(TODAY()&gt;=AB$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8457,42 +8463,42 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I35:AA35">
-    <cfRule type="expression" dxfId="77" priority="622">
+    <cfRule type="expression" dxfId="80" priority="622">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB35">
-    <cfRule type="expression" dxfId="76" priority="629">
+    <cfRule type="expression" dxfId="79" priority="629">
       <formula>AND(TODAY()&gt;=AB$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I41:AA41 I44:AA44 I46:AA46">
-    <cfRule type="expression" dxfId="75" priority="604">
+    <cfRule type="expression" dxfId="78" priority="604">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB41 AB44 AB46">
-    <cfRule type="expression" dxfId="74" priority="611">
+    <cfRule type="expression" dxfId="77" priority="611">
       <formula>AND(TODAY()&gt;=AB$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I57:AA57">
-    <cfRule type="expression" dxfId="73" priority="586">
+    <cfRule type="expression" dxfId="76" priority="586">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB57">
-    <cfRule type="expression" dxfId="72" priority="593">
+    <cfRule type="expression" dxfId="75" priority="593">
       <formula>AND(TODAY()&gt;=AB$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I60:AA60">
-    <cfRule type="expression" dxfId="71" priority="577">
+    <cfRule type="expression" dxfId="74" priority="577">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB60">
-    <cfRule type="expression" dxfId="70" priority="584">
+    <cfRule type="expression" dxfId="73" priority="584">
       <formula>AND(TODAY()&gt;=AB$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8581,22 +8587,22 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I53:AA53">
-    <cfRule type="expression" dxfId="69" priority="561">
+    <cfRule type="expression" dxfId="72" priority="561">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB53">
-    <cfRule type="expression" dxfId="68" priority="568">
+    <cfRule type="expression" dxfId="71" priority="568">
       <formula>AND(TODAY()&gt;=AB$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I54:AA54">
-    <cfRule type="expression" dxfId="67" priority="553">
+    <cfRule type="expression" dxfId="70" priority="553">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB54">
-    <cfRule type="expression" dxfId="66" priority="559">
+    <cfRule type="expression" dxfId="69" priority="559">
       <formula>AND(TODAY()&gt;=AB$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8629,12 +8635,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I31:AA31">
-    <cfRule type="expression" dxfId="65" priority="543">
+    <cfRule type="expression" dxfId="68" priority="543">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB31">
-    <cfRule type="expression" dxfId="64" priority="550">
+    <cfRule type="expression" dxfId="67" priority="550">
       <formula>AND(TODAY()&gt;=AB$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8653,12 +8659,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I33:AA34">
-    <cfRule type="expression" dxfId="63" priority="534">
+    <cfRule type="expression" dxfId="66" priority="534">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB33:AB34">
-    <cfRule type="expression" dxfId="62" priority="541">
+    <cfRule type="expression" dxfId="65" priority="541">
       <formula>AND(TODAY()&gt;=AB$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8677,29 +8683,29 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I19:AA19">
-    <cfRule type="expression" dxfId="61" priority="525">
+    <cfRule type="expression" dxfId="64" priority="525">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB19">
-    <cfRule type="expression" dxfId="60" priority="532">
+    <cfRule type="expression" dxfId="63" priority="532">
       <formula>AND(TODAY()&gt;=AB$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I21:AB21 I44:AB44 I57:AB57">
-    <cfRule type="expression" dxfId="59" priority="810" stopIfTrue="1">
+    <cfRule type="expression" dxfId="62" priority="810" stopIfTrue="1">
       <formula>AND($C21="Risque faible",I$5&gt;=$F22,I$5&lt;=$F22+$G21-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="58" priority="811" stopIfTrue="1">
+    <cfRule type="expression" dxfId="61" priority="811" stopIfTrue="1">
       <formula>AND($C21="Risque élevé",I$5&gt;=$F22,I$5&lt;=$F22+$G21-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="57" priority="812" stopIfTrue="1">
+    <cfRule type="expression" dxfId="60" priority="812" stopIfTrue="1">
       <formula>AND($C21="En bonne voie",I$5&gt;=$F22,I$5&lt;=$F22+$G21-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="56" priority="813" stopIfTrue="1">
+    <cfRule type="expression" dxfId="59" priority="813" stopIfTrue="1">
       <formula>AND($C21="Risque moyen",I$5&gt;=$F22,I$5&lt;=$F22+$G21-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="55" priority="814" stopIfTrue="1">
+    <cfRule type="expression" dxfId="58" priority="814" stopIfTrue="1">
       <formula>AND(LEN($C21)=0,I$5&gt;=$F22,I$5&lt;=$F22+$G21-1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8718,12 +8724,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I36:AA36">
-    <cfRule type="expression" dxfId="54" priority="453">
+    <cfRule type="expression" dxfId="57" priority="453">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB36">
-    <cfRule type="expression" dxfId="53" priority="460">
+    <cfRule type="expression" dxfId="56" priority="460">
       <formula>AND(TODAY()&gt;=AB$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8742,7 +8748,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I22:AA22">
-    <cfRule type="expression" dxfId="52" priority="407">
+    <cfRule type="expression" dxfId="55" priority="407">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8761,12 +8767,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I28:AA29">
-    <cfRule type="expression" dxfId="51" priority="425">
+    <cfRule type="expression" dxfId="54" priority="425">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB28:AB29">
-    <cfRule type="expression" dxfId="50" priority="432">
+    <cfRule type="expression" dxfId="53" priority="432">
       <formula>AND(TODAY()&gt;=AB$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8785,17 +8791,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I26:AA26">
-    <cfRule type="expression" dxfId="49" priority="416">
+    <cfRule type="expression" dxfId="52" priority="416">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB26">
-    <cfRule type="expression" dxfId="48" priority="423">
+    <cfRule type="expression" dxfId="51" priority="423">
       <formula>AND(TODAY()&gt;=AB$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB22">
-    <cfRule type="expression" dxfId="47" priority="414">
+    <cfRule type="expression" dxfId="50" priority="414">
       <formula>AND(TODAY()&gt;=AB$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8814,12 +8820,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I20:AA20">
-    <cfRule type="expression" dxfId="46" priority="398">
+    <cfRule type="expression" dxfId="49" priority="398">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB20">
-    <cfRule type="expression" dxfId="45" priority="405">
+    <cfRule type="expression" dxfId="48" priority="405">
       <formula>AND(TODAY()&gt;=AB$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8838,7 +8844,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I42:AA43">
-    <cfRule type="expression" dxfId="44" priority="335">
+    <cfRule type="expression" dxfId="47" priority="335">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8857,17 +8863,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I38:AA39">
-    <cfRule type="expression" dxfId="43" priority="353">
+    <cfRule type="expression" dxfId="46" priority="353">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB38:AB39">
-    <cfRule type="expression" dxfId="42" priority="360">
+    <cfRule type="expression" dxfId="45" priority="360">
       <formula>AND(TODAY()&gt;=AB$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB42:AB43">
-    <cfRule type="expression" dxfId="41" priority="342">
+    <cfRule type="expression" dxfId="44" priority="342">
       <formula>AND(TODAY()&gt;=AB$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8886,22 +8892,22 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I47:AA49">
-    <cfRule type="expression" dxfId="40" priority="326">
+    <cfRule type="expression" dxfId="43" priority="326">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB47:AB49">
-    <cfRule type="expression" dxfId="39" priority="333">
+    <cfRule type="expression" dxfId="42" priority="333">
       <formula>AND(TODAY()&gt;=AB$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I37:AA37">
-    <cfRule type="expression" dxfId="38" priority="309">
+    <cfRule type="expression" dxfId="41" priority="309">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB37">
-    <cfRule type="expression" dxfId="37" priority="310">
+    <cfRule type="expression" dxfId="40" priority="310">
       <formula>AND(TODAY()&gt;=AB$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8934,12 +8940,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I40:AA40">
-    <cfRule type="expression" dxfId="36" priority="299">
+    <cfRule type="expression" dxfId="39" priority="299">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB40">
-    <cfRule type="expression" dxfId="35" priority="306">
+    <cfRule type="expression" dxfId="38" priority="306">
       <formula>AND(TODAY()&gt;=AB$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8958,12 +8964,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I50:AA52">
-    <cfRule type="expression" dxfId="34" priority="281">
+    <cfRule type="expression" dxfId="37" priority="281">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB50:AB52">
-    <cfRule type="expression" dxfId="33" priority="288">
+    <cfRule type="expression" dxfId="36" priority="288">
       <formula>AND(TODAY()&gt;=AB$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8982,12 +8988,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I55:AA56">
-    <cfRule type="expression" dxfId="32" priority="272">
+    <cfRule type="expression" dxfId="35" priority="272">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB55:AB56">
-    <cfRule type="expression" dxfId="31" priority="279">
+    <cfRule type="expression" dxfId="34" priority="279">
       <formula>AND(TODAY()&gt;=AB$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9006,7 +9012,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I58:AA58">
-    <cfRule type="expression" dxfId="30" priority="217">
+    <cfRule type="expression" dxfId="33" priority="217">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9025,27 +9031,27 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I59:AA59">
-    <cfRule type="expression" dxfId="29" priority="226">
+    <cfRule type="expression" dxfId="32" priority="226">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB59">
-    <cfRule type="expression" dxfId="28" priority="233">
+    <cfRule type="expression" dxfId="31" priority="233">
       <formula>AND(TODAY()&gt;=AB$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB58">
-    <cfRule type="expression" dxfId="27" priority="219">
+    <cfRule type="expression" dxfId="30" priority="219">
       <formula>AND(TODAY()&gt;=AB$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB61">
-    <cfRule type="expression" dxfId="26" priority="165">
+    <cfRule type="expression" dxfId="29" priority="165">
       <formula>AND(TODAY()&gt;=AB$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I61:AA61">
-    <cfRule type="expression" dxfId="25" priority="164">
+    <cfRule type="expression" dxfId="28" priority="164">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9078,22 +9084,22 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I62:AA63">
-    <cfRule type="expression" dxfId="24" priority="118">
+    <cfRule type="expression" dxfId="27" priority="118">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB62:AB63">
-    <cfRule type="expression" dxfId="23" priority="120">
+    <cfRule type="expression" dxfId="26" priority="120">
       <formula>AND(TODAY()&gt;=AB$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I65:AA65">
-    <cfRule type="expression" dxfId="22" priority="101">
+    <cfRule type="expression" dxfId="25" priority="101">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB64">
-    <cfRule type="expression" dxfId="21" priority="111">
+    <cfRule type="expression" dxfId="24" priority="111">
       <formula>AND(TODAY()&gt;=AB$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9126,12 +9132,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I64:AA64">
-    <cfRule type="expression" dxfId="20" priority="109">
+    <cfRule type="expression" dxfId="23" priority="109">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB65">
-    <cfRule type="expression" dxfId="19" priority="102">
+    <cfRule type="expression" dxfId="22" priority="102">
       <formula>AND(TODAY()&gt;=AB$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9150,12 +9156,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I66:AA66">
-    <cfRule type="expression" dxfId="18" priority="91">
+    <cfRule type="expression" dxfId="21" priority="91">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB66">
-    <cfRule type="expression" dxfId="17" priority="93">
+    <cfRule type="expression" dxfId="20" priority="93">
       <formula>AND(TODAY()&gt;=AB$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9174,17 +9180,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I67:AA67">
-    <cfRule type="expression" dxfId="16" priority="82">
+    <cfRule type="expression" dxfId="19" priority="82">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB67">
-    <cfRule type="expression" dxfId="15" priority="84">
+    <cfRule type="expression" dxfId="18" priority="84">
       <formula>AND(TODAY()&gt;=AB$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I68:AA68">
-    <cfRule type="expression" dxfId="14" priority="74">
+    <cfRule type="expression" dxfId="17" priority="74">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9203,7 +9209,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB68">
-    <cfRule type="expression" dxfId="13" priority="75">
+    <cfRule type="expression" dxfId="16" priority="75">
       <formula>AND(TODAY()&gt;=AB$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9222,29 +9228,29 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I45:AA45">
-    <cfRule type="expression" dxfId="12" priority="55">
+    <cfRule type="expression" dxfId="15" priority="55">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB45">
-    <cfRule type="expression" dxfId="11" priority="62">
+    <cfRule type="expression" dxfId="14" priority="62">
       <formula>AND(TODAY()&gt;=AB$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I23:AB23">
-    <cfRule type="expression" dxfId="10" priority="995" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="995" stopIfTrue="1">
       <formula>AND($C23="Risque faible",I$5&gt;=$F25,I$5&lt;=$F25+$G23-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="996" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="996" stopIfTrue="1">
       <formula>AND($C23="Risque élevé",I$5&gt;=$F25,I$5&lt;=$F25+$G23-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="997" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="997" stopIfTrue="1">
       <formula>AND($C23="En bonne voie",I$5&gt;=$F25,I$5&lt;=$F25+$G23-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="998" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="998" stopIfTrue="1">
       <formula>AND($C23="Risque moyen",I$5&gt;=$F25,I$5&lt;=$F25+$G23-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="999" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="999" stopIfTrue="1">
       <formula>AND(LEN($C23)=0,I$5&gt;=$F25,I$5&lt;=$F25+$G23-1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9263,12 +9269,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I24:AA25">
-    <cfRule type="expression" dxfId="5" priority="28">
+    <cfRule type="expression" dxfId="8" priority="28">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB24:AB25">
-    <cfRule type="expression" dxfId="4" priority="30">
+    <cfRule type="expression" dxfId="7" priority="30">
       <formula>AND(TODAY()&gt;=AB$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9287,12 +9293,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I52:AA52">
-    <cfRule type="expression" dxfId="3" priority="10">
+    <cfRule type="expression" dxfId="6" priority="10">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB52">
-    <cfRule type="expression" dxfId="2" priority="12">
+    <cfRule type="expression" dxfId="5" priority="12">
       <formula>AND(TODAY()&gt;=AB$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9311,12 +9317,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I34:AA34">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="4" priority="1">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB34">
-    <cfRule type="expression" dxfId="0" priority="3">
+    <cfRule type="expression" dxfId="3" priority="3">
       <formula>AND(TODAY()&gt;=AB$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9956,6 +9962,36 @@
           <xm:sqref>E24:E25</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{A63CCB1F-A7A9-FB4D-96BE-C68735FCF745}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>E52</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{77136285-CE6D-CC44-A948-A1CCC3E96272}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>E34</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="786" id="{628A03C6-EE71-4B44-A6BA-69DC45906EA6}">
             <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
               <x14:cfvo type="percent">
@@ -10716,21 +10752,6 @@
           <xm:sqref>I24:AB25</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{A63CCB1F-A7A9-FB4D-96BE-C68735FCF745}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="num">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>E52</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="13" id="{E15BFD62-9391-FA42-8B09-20ECBD2428FD}">
             <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
               <x14:cfvo type="percent">
@@ -10748,21 +10769,6 @@
             </x14:iconSet>
           </x14:cfRule>
           <xm:sqref>I52:AB52</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{77136285-CE6D-CC44-A948-A1CCC3E96272}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="num">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>E34</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="4" id="{A5B4E9B3-6226-4145-BD2D-873C36B43997}">

</xml_diff>

<commit_message>
MAJ plannification, ajustement du mouvement de LR à partir d'une échelle
</commit_message>
<xml_diff>
--- a/Diagramme_de_Gantt.xlsx
+++ b/Diagramme_de_Gantt.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67153CC9-9E1E-BD4A-B685-8F0F2BA4F06D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A256A19-B1F7-3F42-A12B-76DFABF3D71A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="460" windowWidth="38400" windowHeight="21140" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16400" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt" sheetId="11" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="94">
   <si>
     <t>Créez un diagramme de Gantt dans cette feuille de calcul.
 Entrez le titre de ce projet dans la cellule B1. 
@@ -3985,8 +3985,8 @@
   </sheetPr>
   <dimension ref="A1:AB71"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A38" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6798,13 +6798,13 @@
         <v>66</v>
       </c>
       <c r="C43" s="33" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D43" s="33" t="s">
         <v>46</v>
       </c>
       <c r="E43" s="30">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="F43" s="31">
         <v>43894</v>
@@ -7190,11 +7190,13 @@
         <v>74</v>
       </c>
       <c r="C50" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="D50" s="33"/>
+        <v>16</v>
+      </c>
+      <c r="D50" s="33" t="s">
+        <v>46</v>
+      </c>
       <c r="E50" s="30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F50" s="31">
         <v>43896</v>
@@ -7499,10 +7501,10 @@
         <v>16</v>
       </c>
       <c r="D55" s="33" t="s">
-        <v>46</v>
+        <v>90</v>
       </c>
       <c r="E55" s="30">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="F55" s="31">
         <v>43896</v>
@@ -7604,7 +7606,7 @@
         <v>46</v>
       </c>
       <c r="E56" s="30">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="F56" s="31">
         <v>43894</v>
@@ -7738,7 +7740,7 @@
         <v>90</v>
       </c>
       <c r="E58" s="30">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="F58" s="31">
         <v>43894</v>

</xml_diff>

<commit_message>
Relacher lingots aleatoirement, MaJ Calendrier, épuration de code
</commit_message>
<xml_diff>
--- a/Diagramme_de_Gantt.xlsx
+++ b/Diagramme_de_Gantt.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{785C754E-9115-CD4E-B8D3-D02BE0B7CDCC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B573F8B3-CED5-4A22-9485-05E3918E6823}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16400" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt" sheetId="11" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="94">
   <si>
     <t>Créez un diagramme de Gantt dans cette feuille de calcul.
 Entrez le titre de ce projet dans la cellule B1. 
@@ -3985,25 +3985,25 @@
   </sheetPr>
   <dimension ref="A1:AB71"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A44" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A37" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="I51" sqref="I51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" style="14" customWidth="1"/>
-    <col min="2" max="2" width="32.5" customWidth="1"/>
-    <col min="3" max="3" width="14.83203125" style="20" customWidth="1"/>
-    <col min="4" max="4" width="20.5" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" customWidth="1"/>
-    <col min="6" max="6" width="11.1640625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="10.5" customWidth="1"/>
-    <col min="8" max="8" width="2.6640625" customWidth="1"/>
-    <col min="9" max="28" width="9.33203125" customWidth="1"/>
-    <col min="33" max="34" width="10.33203125"/>
+    <col min="1" max="1" width="2.7109375" style="14" customWidth="1"/>
+    <col min="2" max="2" width="32.42578125" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" style="20" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" customWidth="1"/>
+    <col min="8" max="8" width="2.7109375" customWidth="1"/>
+    <col min="9" max="28" width="9.28515625" customWidth="1"/>
+    <col min="33" max="34" width="10.28515625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -4037,7 +4037,7 @@
       <c r="AA1" s="20"/>
       <c r="AB1" s="20"/>
     </row>
-    <row r="2" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
         <v>1</v>
       </c>
@@ -4073,7 +4073,7 @@
       </c>
       <c r="AB2" s="65"/>
     </row>
-    <row r="3" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>2</v>
       </c>
@@ -4091,7 +4091,7 @@
       <c r="G3" s="70"/>
       <c r="H3" s="22"/>
     </row>
-    <row r="4" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="15" t="s">
         <v>3</v>
       </c>
@@ -4132,7 +4132,7 @@
       <c r="AA4" s="40"/>
       <c r="AB4" s="40"/>
     </row>
-    <row r="5" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>4</v>
       </c>
@@ -4224,7 +4224,7 @@
         <v>43899</v>
       </c>
     </row>
-    <row r="6" spans="1:28" s="20" customFormat="1" ht="25.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:28" s="20" customFormat="1" ht="25.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>5</v>
       </c>
@@ -4256,7 +4256,7 @@
       <c r="AA6" s="43"/>
       <c r="AB6" s="43"/>
     </row>
-    <row r="7" spans="1:28" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" ht="30.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="15" t="s">
         <v>6</v>
       </c>
@@ -4360,7 +4360,7 @@
         <v>l</v>
       </c>
     </row>
-    <row r="8" spans="1:28" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="14" t="s">
         <v>7</v>
       </c>
@@ -4390,7 +4390,7 @@
       <c r="AA8" s="35"/>
       <c r="AB8" s="35"/>
     </row>
-    <row r="9" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>8</v>
       </c>
@@ -4494,7 +4494,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="15"/>
       <c r="B10" s="54" t="s">
         <v>30</v>
@@ -4588,7 +4588,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="15"/>
       <c r="B11" s="50" t="s">
         <v>31</v>
@@ -4690,7 +4690,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="14"/>
       <c r="B12" s="50" t="s">
         <v>32</v>
@@ -4792,7 +4792,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="14"/>
       <c r="B13" s="50" t="s">
         <v>33</v>
@@ -4894,7 +4894,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="15"/>
       <c r="B14" s="54" t="s">
         <v>34</v>
@@ -4986,7 +4986,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="15"/>
       <c r="B15" s="50" t="s">
         <v>35</v>
@@ -5088,7 +5088,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="15"/>
       <c r="B16" s="50" t="s">
         <v>36</v>
@@ -5190,7 +5190,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="14"/>
       <c r="B17" s="54" t="s">
         <v>37</v>
@@ -5282,7 +5282,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="14"/>
       <c r="B18" s="50" t="s">
         <v>38</v>
@@ -5374,7 +5374,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="14"/>
       <c r="B19" s="53" t="s">
         <v>54</v>
@@ -5416,7 +5416,7 @@
       <c r="AA19" s="37"/>
       <c r="AB19" s="37"/>
     </row>
-    <row r="20" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="14"/>
       <c r="B20" s="53" t="s">
         <v>55</v>
@@ -5458,7 +5458,7 @@
       <c r="AA20" s="37"/>
       <c r="AB20" s="37"/>
     </row>
-    <row r="21" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="14"/>
       <c r="B21" s="50" t="s">
         <v>39</v>
@@ -5550,7 +5550,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="14"/>
       <c r="B22" s="53" t="s">
         <v>56</v>
@@ -5592,7 +5592,7 @@
       <c r="AA22" s="37"/>
       <c r="AB22" s="37"/>
     </row>
-    <row r="23" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="14"/>
       <c r="B23" s="50" t="s">
         <v>59</v>
@@ -5684,7 +5684,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="14"/>
       <c r="B24" s="53" t="s">
         <v>91</v>
@@ -5726,7 +5726,7 @@
       <c r="AA24" s="37"/>
       <c r="AB24" s="37"/>
     </row>
-    <row r="25" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="14"/>
       <c r="B25" s="53" t="s">
         <v>57</v>
@@ -5768,7 +5768,7 @@
       <c r="AA25" s="37"/>
       <c r="AB25" s="37"/>
     </row>
-    <row r="26" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="14"/>
       <c r="B26" s="53" t="s">
         <v>58</v>
@@ -5810,7 +5810,7 @@
       <c r="AA26" s="37"/>
       <c r="AB26" s="37"/>
     </row>
-    <row r="27" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="14"/>
       <c r="B27" s="50" t="s">
         <v>40</v>
@@ -5902,7 +5902,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="14"/>
       <c r="B28" s="53" t="s">
         <v>60</v>
@@ -5944,7 +5944,7 @@
       <c r="AA28" s="37"/>
       <c r="AB28" s="37"/>
     </row>
-    <row r="29" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="14"/>
       <c r="B29" s="53" t="s">
         <v>61</v>
@@ -5986,7 +5986,7 @@
       <c r="AA29" s="37"/>
       <c r="AB29" s="37"/>
     </row>
-    <row r="30" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="14"/>
       <c r="B30" s="50" t="s">
         <v>41</v>
@@ -6088,7 +6088,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="14"/>
       <c r="B31" s="50" t="s">
         <v>52</v>
@@ -6120,7 +6120,7 @@
       <c r="AA31" s="37"/>
       <c r="AB31" s="37"/>
     </row>
-    <row r="32" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="14"/>
       <c r="B32" s="53" t="s">
         <v>51</v>
@@ -6222,7 +6222,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:28" s="64" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:28" s="64" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="56"/>
       <c r="B33" s="57" t="s">
         <v>53</v>
@@ -6264,7 +6264,7 @@
       <c r="AA33" s="63"/>
       <c r="AB33" s="63"/>
     </row>
-    <row r="34" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="14"/>
       <c r="B34" s="50" t="s">
         <v>93</v>
@@ -6306,7 +6306,7 @@
       <c r="AA34" s="37"/>
       <c r="AB34" s="37"/>
     </row>
-    <row r="35" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="14"/>
       <c r="B35" s="54" t="s">
         <v>42</v>
@@ -6398,7 +6398,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="14"/>
       <c r="B36" s="50" t="s">
         <v>62</v>
@@ -6440,7 +6440,7 @@
       <c r="AA36" s="37"/>
       <c r="AB36" s="37"/>
     </row>
-    <row r="37" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="14"/>
       <c r="B37" s="50" t="s">
         <v>43</v>
@@ -6532,7 +6532,7 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:28" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:28" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="14"/>
       <c r="B38" s="53" t="s">
         <v>63</v>
@@ -6574,7 +6574,7 @@
       <c r="AA38" s="37"/>
       <c r="AB38" s="37"/>
     </row>
-    <row r="39" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="14"/>
       <c r="B39" s="53" t="s">
         <v>64</v>
@@ -6616,7 +6616,7 @@
       <c r="AA39" s="37"/>
       <c r="AB39" s="37"/>
     </row>
-    <row r="40" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="14"/>
       <c r="B40" s="53" t="s">
         <v>72</v>
@@ -6658,7 +6658,7 @@
       <c r="AA40" s="37"/>
       <c r="AB40" s="37"/>
     </row>
-    <row r="41" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="14"/>
       <c r="B41" s="50" t="s">
         <v>44</v>
@@ -6750,7 +6750,7 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:28" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:28" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="14"/>
       <c r="B42" s="53" t="s">
         <v>65</v>
@@ -6792,7 +6792,7 @@
       <c r="AA42" s="37"/>
       <c r="AB42" s="37"/>
     </row>
-    <row r="43" spans="1:28" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:28" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="14"/>
       <c r="B43" s="53" t="s">
         <v>66</v>
@@ -6834,7 +6834,7 @@
       <c r="AA43" s="37"/>
       <c r="AB43" s="37"/>
     </row>
-    <row r="44" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="14"/>
       <c r="B44" s="50" t="s">
         <v>40</v>
@@ -6926,7 +6926,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="14"/>
       <c r="B45" s="53" t="s">
         <v>67</v>
@@ -6968,7 +6968,7 @@
       <c r="AA45" s="37"/>
       <c r="AB45" s="37"/>
     </row>
-    <row r="46" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="14"/>
       <c r="B46" s="50" t="s">
         <v>68</v>
@@ -7060,7 +7060,7 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:28" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:28" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="14"/>
       <c r="B47" s="53" t="s">
         <v>69</v>
@@ -7102,7 +7102,7 @@
       <c r="AA47" s="37"/>
       <c r="AB47" s="37"/>
     </row>
-    <row r="48" spans="1:28" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:28" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="14"/>
       <c r="B48" s="53" t="s">
         <v>70</v>
@@ -7144,7 +7144,7 @@
       <c r="AA48" s="37"/>
       <c r="AB48" s="37"/>
     </row>
-    <row r="49" spans="1:28" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:28" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="14"/>
       <c r="B49" s="53" t="s">
         <v>71</v>
@@ -7186,7 +7186,7 @@
       <c r="AA49" s="37"/>
       <c r="AB49" s="37"/>
     </row>
-    <row r="50" spans="1:28" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:28" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="14"/>
       <c r="B50" s="53" t="s">
         <v>74</v>
@@ -7228,17 +7228,19 @@
       <c r="AA50" s="37"/>
       <c r="AB50" s="37"/>
     </row>
-    <row r="51" spans="1:28" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:28" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="14"/>
       <c r="B51" s="53" t="s">
         <v>73</v>
       </c>
       <c r="C51" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="D51" s="33"/>
+        <v>16</v>
+      </c>
+      <c r="D51" s="33" t="s">
+        <v>89</v>
+      </c>
       <c r="E51" s="30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F51" s="31">
         <v>43896</v>
@@ -7268,7 +7270,7 @@
       <c r="AA51" s="37"/>
       <c r="AB51" s="37"/>
     </row>
-    <row r="52" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="14"/>
       <c r="B52" s="50" t="s">
         <v>92</v>
@@ -7310,7 +7312,7 @@
       <c r="AA52" s="37"/>
       <c r="AB52" s="37"/>
     </row>
-    <row r="53" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="14"/>
       <c r="B53" s="54" t="s">
         <v>75</v>
@@ -7402,7 +7404,7 @@
         <v/>
       </c>
     </row>
-    <row r="54" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="14"/>
       <c r="B54" s="50" t="s">
         <v>76</v>
@@ -7494,7 +7496,7 @@
         <v/>
       </c>
     </row>
-    <row r="55" spans="1:28" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:28" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="14"/>
       <c r="B55" s="53" t="s">
         <v>77</v>
@@ -7596,7 +7598,7 @@
         <v/>
       </c>
     </row>
-    <row r="56" spans="1:28" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:28" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="14"/>
       <c r="B56" s="53" t="s">
         <v>78</v>
@@ -7638,7 +7640,7 @@
       <c r="AA56" s="37"/>
       <c r="AB56" s="37"/>
     </row>
-    <row r="57" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="14"/>
       <c r="B57" s="50" t="s">
         <v>80</v>
@@ -7730,13 +7732,13 @@
         <v/>
       </c>
     </row>
-    <row r="58" spans="1:28" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:28" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="14"/>
       <c r="B58" s="53" t="s">
         <v>79</v>
       </c>
       <c r="C58" s="33" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D58" s="33" t="s">
         <v>90</v>
@@ -7772,7 +7774,7 @@
       <c r="AA58" s="37"/>
       <c r="AB58" s="37"/>
     </row>
-    <row r="59" spans="1:28" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:28" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="14"/>
       <c r="B59" s="53" t="s">
         <v>81</v>
@@ -7814,7 +7816,7 @@
       <c r="AA59" s="37"/>
       <c r="AB59" s="37"/>
     </row>
-    <row r="60" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="14"/>
       <c r="B60" s="50" t="s">
         <v>45</v>
@@ -7856,7 +7858,7 @@
       <c r="AA60" s="37"/>
       <c r="AB60" s="37"/>
     </row>
-    <row r="61" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="14"/>
       <c r="B61" s="50" t="s">
         <v>82</v>
@@ -7888,7 +7890,7 @@
       <c r="AA61" s="37"/>
       <c r="AB61" s="37"/>
     </row>
-    <row r="62" spans="1:28" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:28" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="14"/>
       <c r="B62" s="53" t="s">
         <v>83</v>
@@ -7930,7 +7932,7 @@
       <c r="AA62" s="37"/>
       <c r="AB62" s="37"/>
     </row>
-    <row r="63" spans="1:28" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:28" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="14"/>
       <c r="B63" s="53" t="s">
         <v>84</v>
@@ -7972,7 +7974,7 @@
       <c r="AA63" s="37"/>
       <c r="AB63" s="37"/>
     </row>
-    <row r="64" spans="1:28" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:28" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="14"/>
       <c r="B64" s="53" t="s">
         <v>85</v>
@@ -8014,7 +8016,7 @@
       <c r="AA64" s="37"/>
       <c r="AB64" s="37"/>
     </row>
-    <row r="65" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="14"/>
       <c r="B65" s="50" t="s">
         <v>86</v>
@@ -8046,7 +8048,7 @@
       <c r="AA65" s="37"/>
       <c r="AB65" s="37"/>
     </row>
-    <row r="66" spans="1:28" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:28" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="14"/>
       <c r="B66" s="53" t="s">
         <v>87</v>
@@ -8088,7 +8090,7 @@
       <c r="AA66" s="37"/>
       <c r="AB66" s="37"/>
     </row>
-    <row r="67" spans="1:28" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:28" s="2" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="14"/>
       <c r="B67" s="53" t="s">
         <v>88</v>
@@ -8130,7 +8132,7 @@
       <c r="AA67" s="37"/>
       <c r="AB67" s="37"/>
     </row>
-    <row r="68" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="14"/>
       <c r="B68" s="50"/>
       <c r="C68" s="33"/>
@@ -8160,7 +8162,7 @@
       <c r="AA68" s="37"/>
       <c r="AB68" s="37"/>
     </row>
-    <row r="69" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:28" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="15" t="s">
         <v>9</v>
       </c>
@@ -8194,12 +8196,12 @@
       <c r="AA69" s="36"/>
       <c r="AB69" s="36"/>
     </row>
-    <row r="70" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D70" s="5"/>
       <c r="G70" s="16"/>
       <c r="H70" s="4"/>
     </row>
-    <row r="71" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D71" s="6"/>
     </row>
   </sheetData>
@@ -10807,13 +10809,13 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="87.1640625" style="10" customWidth="1"/>
-    <col min="2" max="16384" width="9.1640625" style="8"/>
+    <col min="1" max="1" width="87.140625" style="10" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="9" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" s="9" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="11" t="s">
         <v>24</v>
       </c>
@@ -10828,7 +10830,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:1" s="10" customFormat="1" ht="222" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1" s="10" customFormat="1" ht="222" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>27</v>
       </c>

</xml_diff>